<commit_message>
működő Sopron ospf_ következik az asa, vpn
</commit_message>
<xml_diff>
--- a/IP_cim_kiosztas_akutális.xlsx
+++ b/IP_cim_kiosztas_akutális.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Üzemeltető\Vizsgaremek\Uzemelteto_vizsgaremek_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B34DD66-FAF7-4C48-A6EB-D1C9DF97FC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA5EB10-9D47-4DC3-823E-9D57D50F4F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="2760" windowWidth="15180" windowHeight="9300" activeTab="1" xr2:uid="{5DEB228F-9A24-4144-85FF-8E6948A8BA71}"/>
+    <workbookView xWindow="1455" yWindow="2760" windowWidth="20820" windowHeight="9300" activeTab="2" xr2:uid="{5DEB228F-9A24-4144-85FF-8E6948A8BA71}"/>
   </bookViews>
   <sheets>
     <sheet name="Központi Iroda" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="311">
   <si>
     <t>Központi Iroda</t>
   </si>
@@ -772,9 +772,6 @@
     <t>192.168.5.190</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>GigabitEthernet0/1</t>
   </si>
   <si>
@@ -962,6 +959,15 @@
   </si>
   <si>
     <t>0.0.0.63</t>
+  </si>
+  <si>
+    <t>130.10.10.13</t>
+  </si>
+  <si>
+    <t>et0/0</t>
+  </si>
+  <si>
+    <t>130.10.10.14</t>
   </si>
 </sst>
 </file>
@@ -1784,7 +1790,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2078,15 +2084,63 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2099,110 +2153,68 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2210,6 +2222,24 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2219,31 +2249,16 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2601,20 +2616,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="40.5" customHeight="1" thickBot="1">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="124" t="s">
+      <c r="B2" s="116" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -2623,7 +2638,7 @@
       <c r="D2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="129" t="s">
+      <c r="E2" s="121" t="s">
         <v>55</v>
       </c>
       <c r="F2" s="14" t="s">
@@ -2631,13 +2646,13 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="123"/>
-      <c r="B3" s="125"/>
-      <c r="C3" s="126" t="s">
+      <c r="A3" s="115"/>
+      <c r="B3" s="117"/>
+      <c r="C3" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="127"/>
-      <c r="E3" s="130"/>
+      <c r="D3" s="119"/>
+      <c r="E3" s="122"/>
       <c r="F3" s="15" t="s">
         <v>6</v>
       </c>
@@ -2645,10 +2660,10 @@
     <row r="4" spans="1:18" ht="15" customHeight="1">
       <c r="A4" s="40"/>
       <c r="B4" s="24" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>142</v>
@@ -2657,14 +2672,14 @@
       <c r="F4" s="28"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1">
-      <c r="A5" s="119" t="s">
+      <c r="A5" s="111" t="s">
         <v>139</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D5" s="28" t="s">
         <v>142</v>
@@ -2673,7 +2688,7 @@
       <c r="F5" s="25"/>
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1">
-      <c r="A6" s="119"/>
+      <c r="A6" s="111"/>
       <c r="B6" s="1" t="s">
         <v>153</v>
       </c>
@@ -2696,7 +2711,7 @@
       <c r="Q6" s="17"/>
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1">
-      <c r="A7" s="119"/>
+      <c r="A7" s="111"/>
       <c r="B7" s="1" t="s">
         <v>154</v>
       </c>
@@ -2719,7 +2734,7 @@
       <c r="Q7" s="17"/>
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1">
-      <c r="A8" s="118" t="s">
+      <c r="A8" s="110" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="26"/>
@@ -2738,7 +2753,7 @@
       <c r="Q8" s="17"/>
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1">
-      <c r="A9" s="128"/>
+      <c r="A9" s="120"/>
       <c r="B9" s="26"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -2755,7 +2770,7 @@
       <c r="Q9" s="17"/>
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1">
-      <c r="A10" s="118" t="s">
+      <c r="A10" s="110" t="s">
         <v>155</v>
       </c>
       <c r="B10" s="27" t="s">
@@ -2780,7 +2795,7 @@
       <c r="Q10" s="17"/>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" thickBot="1">
-      <c r="A11" s="119"/>
+      <c r="A11" s="111"/>
       <c r="B11" s="27" t="s">
         <v>158</v>
       </c>
@@ -2794,7 +2809,7 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1">
-      <c r="A12" s="119"/>
+      <c r="A12" s="111"/>
       <c r="B12" s="27" t="s">
         <v>160</v>
       </c>
@@ -2806,39 +2821,39 @@
       </c>
       <c r="E12" s="28"/>
       <c r="F12" s="8"/>
-      <c r="I12" s="116" t="s">
+      <c r="I12" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="112" t="s">
+      <c r="J12" s="128" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="112" t="s">
+      <c r="K12" s="128" t="s">
         <v>18</v>
       </c>
-      <c r="L12" s="112" t="s">
+      <c r="L12" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="M12" s="112" t="s">
+      <c r="M12" s="128" t="s">
         <v>20</v>
       </c>
-      <c r="N12" s="112" t="s">
+      <c r="N12" s="128" t="s">
         <v>21</v>
       </c>
-      <c r="O12" s="112" t="s">
+      <c r="O12" s="128" t="s">
         <v>22</v>
       </c>
-      <c r="P12" s="112" t="s">
+      <c r="P12" s="128" t="s">
         <v>23</v>
       </c>
-      <c r="Q12" s="112" t="s">
+      <c r="Q12" s="128" t="s">
         <v>55</v>
       </c>
-      <c r="R12" s="114" t="s">
+      <c r="R12" s="130" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1">
-      <c r="A13" s="119"/>
+      <c r="A13" s="111"/>
       <c r="B13" s="27" t="s">
         <v>162</v>
       </c>
@@ -2850,19 +2865,19 @@
       </c>
       <c r="E13" s="28"/>
       <c r="F13" s="8"/>
-      <c r="I13" s="117"/>
-      <c r="J13" s="113"/>
-      <c r="K13" s="113"/>
-      <c r="L13" s="113"/>
-      <c r="M13" s="113"/>
-      <c r="N13" s="113"/>
-      <c r="O13" s="113"/>
-      <c r="P13" s="113"/>
-      <c r="Q13" s="113"/>
-      <c r="R13" s="115"/>
+      <c r="I13" s="127"/>
+      <c r="J13" s="129"/>
+      <c r="K13" s="129"/>
+      <c r="L13" s="129"/>
+      <c r="M13" s="129"/>
+      <c r="N13" s="129"/>
+      <c r="O13" s="129"/>
+      <c r="P13" s="129"/>
+      <c r="Q13" s="129"/>
+      <c r="R13" s="131"/>
     </row>
     <row r="14" spans="1:18" ht="15" customHeight="1">
-      <c r="A14" s="119"/>
+      <c r="A14" s="111"/>
       <c r="B14" s="27" t="s">
         <v>164</v>
       </c>
@@ -2874,113 +2889,113 @@
       </c>
       <c r="E14" s="28"/>
       <c r="F14" s="8"/>
-      <c r="I14" s="109" t="s">
+      <c r="I14" s="124" t="s">
         <v>33</v>
       </c>
-      <c r="J14" s="109">
+      <c r="J14" s="124">
         <v>7</v>
       </c>
-      <c r="K14" s="109">
+      <c r="K14" s="124">
         <v>30</v>
       </c>
-      <c r="L14" s="110" t="s">
+      <c r="L14" s="123" t="s">
         <v>39</v>
       </c>
-      <c r="M14" s="109" t="s">
+      <c r="M14" s="124" t="s">
         <v>31</v>
       </c>
-      <c r="N14" s="111" t="s">
+      <c r="N14" s="125" t="s">
         <v>38</v>
       </c>
-      <c r="O14" s="110" t="s">
+      <c r="O14" s="123" t="s">
         <v>40</v>
       </c>
-      <c r="P14" s="110" t="s">
+      <c r="P14" s="123" t="s">
         <v>41</v>
       </c>
-      <c r="Q14" s="110" t="s">
+      <c r="Q14" s="123" t="s">
         <v>51</v>
       </c>
-      <c r="R14" s="110" t="s">
+      <c r="R14" s="123" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="15" customHeight="1">
-      <c r="A15" s="119"/>
+      <c r="A15" s="111"/>
       <c r="B15" s="27"/>
       <c r="C15" s="28"/>
       <c r="D15" s="28"/>
       <c r="E15" s="28"/>
       <c r="F15" s="8"/>
-      <c r="I15" s="109"/>
-      <c r="J15" s="109"/>
-      <c r="K15" s="109"/>
-      <c r="L15" s="110"/>
-      <c r="M15" s="109"/>
-      <c r="N15" s="111"/>
-      <c r="O15" s="110"/>
-      <c r="P15" s="110"/>
-      <c r="Q15" s="110"/>
-      <c r="R15" s="110"/>
+      <c r="I15" s="124"/>
+      <c r="J15" s="124"/>
+      <c r="K15" s="124"/>
+      <c r="L15" s="123"/>
+      <c r="M15" s="124"/>
+      <c r="N15" s="125"/>
+      <c r="O15" s="123"/>
+      <c r="P15" s="123"/>
+      <c r="Q15" s="123"/>
+      <c r="R15" s="123"/>
     </row>
     <row r="16" spans="1:18" ht="15" customHeight="1">
-      <c r="A16" s="119"/>
+      <c r="A16" s="111"/>
       <c r="B16" s="27"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="8"/>
-      <c r="I16" s="109" t="s">
+      <c r="I16" s="124" t="s">
         <v>34</v>
       </c>
-      <c r="J16" s="109">
+      <c r="J16" s="124">
         <v>5</v>
       </c>
-      <c r="K16" s="109">
+      <c r="K16" s="124">
         <v>30</v>
       </c>
-      <c r="L16" s="110" t="s">
+      <c r="L16" s="123" t="s">
         <v>42</v>
       </c>
-      <c r="M16" s="109" t="s">
+      <c r="M16" s="124" t="s">
         <v>31</v>
       </c>
-      <c r="N16" s="111" t="s">
+      <c r="N16" s="125" t="s">
         <v>38</v>
       </c>
-      <c r="O16" s="110" t="s">
+      <c r="O16" s="123" t="s">
         <v>43</v>
       </c>
-      <c r="P16" s="110" t="s">
+      <c r="P16" s="123" t="s">
         <v>44</v>
       </c>
-      <c r="Q16" s="110" t="s">
+      <c r="Q16" s="123" t="s">
         <v>52</v>
       </c>
-      <c r="R16" s="110" t="s">
+      <c r="R16" s="123" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="15" customHeight="1">
-      <c r="A17" s="119"/>
+      <c r="A17" s="111"/>
       <c r="B17" s="27"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="8"/>
-      <c r="I17" s="109"/>
-      <c r="J17" s="109"/>
-      <c r="K17" s="109"/>
-      <c r="L17" s="110"/>
-      <c r="M17" s="109"/>
-      <c r="N17" s="111"/>
-      <c r="O17" s="110"/>
-      <c r="P17" s="110"/>
-      <c r="Q17" s="110"/>
-      <c r="R17" s="110"/>
+      <c r="I17" s="124"/>
+      <c r="J17" s="124"/>
+      <c r="K17" s="124"/>
+      <c r="L17" s="123"/>
+      <c r="M17" s="124"/>
+      <c r="N17" s="125"/>
+      <c r="O17" s="123"/>
+      <c r="P17" s="123"/>
+      <c r="Q17" s="123"/>
+      <c r="R17" s="123"/>
     </row>
     <row r="18" spans="1:18" ht="15" customHeight="1">
-      <c r="A18" s="118" t="s">
+      <c r="A18" s="110" t="s">
         <v>166</v>
       </c>
       <c r="B18" s="27" t="s">
@@ -2994,39 +3009,39 @@
       </c>
       <c r="E18" s="28"/>
       <c r="F18" s="8"/>
-      <c r="I18" s="109" t="s">
+      <c r="I18" s="124" t="s">
         <v>35</v>
       </c>
-      <c r="J18" s="109">
+      <c r="J18" s="124">
         <v>1</v>
       </c>
-      <c r="K18" s="109">
+      <c r="K18" s="124">
         <v>6</v>
       </c>
-      <c r="L18" s="110" t="s">
+      <c r="L18" s="123" t="s">
         <v>45</v>
       </c>
-      <c r="M18" s="109" t="s">
+      <c r="M18" s="124" t="s">
         <v>26</v>
       </c>
-      <c r="N18" s="111" t="s">
+      <c r="N18" s="125" t="s">
         <v>37</v>
       </c>
-      <c r="O18" s="110" t="s">
+      <c r="O18" s="123" t="s">
         <v>46</v>
       </c>
-      <c r="P18" s="110" t="s">
+      <c r="P18" s="123" t="s">
         <v>47</v>
       </c>
-      <c r="Q18" s="110" t="s">
+      <c r="Q18" s="123" t="s">
         <v>53</v>
       </c>
-      <c r="R18" s="110" t="s">
+      <c r="R18" s="123" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="15" customHeight="1">
-      <c r="A19" s="119"/>
+      <c r="A19" s="111"/>
       <c r="B19" s="27" t="s">
         <v>158</v>
       </c>
@@ -3038,19 +3053,19 @@
       </c>
       <c r="E19" s="28"/>
       <c r="F19" s="8"/>
-      <c r="I19" s="109"/>
-      <c r="J19" s="109"/>
-      <c r="K19" s="109"/>
-      <c r="L19" s="110"/>
-      <c r="M19" s="109"/>
-      <c r="N19" s="111"/>
-      <c r="O19" s="110"/>
-      <c r="P19" s="110"/>
-      <c r="Q19" s="110"/>
-      <c r="R19" s="110"/>
+      <c r="I19" s="124"/>
+      <c r="J19" s="124"/>
+      <c r="K19" s="124"/>
+      <c r="L19" s="123"/>
+      <c r="M19" s="124"/>
+      <c r="N19" s="125"/>
+      <c r="O19" s="123"/>
+      <c r="P19" s="123"/>
+      <c r="Q19" s="123"/>
+      <c r="R19" s="123"/>
     </row>
     <row r="20" spans="1:18" ht="15" customHeight="1">
-      <c r="A20" s="119"/>
+      <c r="A20" s="111"/>
       <c r="B20" s="27" t="s">
         <v>160</v>
       </c>
@@ -3062,39 +3077,39 @@
       </c>
       <c r="E20" s="28"/>
       <c r="F20" s="8"/>
-      <c r="I20" s="109" t="s">
+      <c r="I20" s="124" t="s">
         <v>36</v>
       </c>
-      <c r="J20" s="109">
+      <c r="J20" s="124">
         <v>1</v>
       </c>
-      <c r="K20" s="109">
+      <c r="K20" s="124">
         <v>6</v>
       </c>
-      <c r="L20" s="110" t="s">
+      <c r="L20" s="123" t="s">
         <v>48</v>
       </c>
-      <c r="M20" s="109" t="s">
+      <c r="M20" s="124" t="s">
         <v>26</v>
       </c>
-      <c r="N20" s="111" t="s">
+      <c r="N20" s="125" t="s">
         <v>37</v>
       </c>
-      <c r="O20" s="110" t="s">
+      <c r="O20" s="123" t="s">
         <v>49</v>
       </c>
-      <c r="P20" s="110" t="s">
+      <c r="P20" s="123" t="s">
         <v>50</v>
       </c>
-      <c r="Q20" s="110" t="s">
+      <c r="Q20" s="123" t="s">
         <v>54</v>
       </c>
-      <c r="R20" s="110" t="s">
+      <c r="R20" s="123" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="15" customHeight="1">
-      <c r="A21" s="119"/>
+      <c r="A21" s="111"/>
       <c r="B21" s="27" t="s">
         <v>162</v>
       </c>
@@ -3106,19 +3121,19 @@
       </c>
       <c r="E21" s="28"/>
       <c r="F21" s="8"/>
-      <c r="I21" s="109"/>
-      <c r="J21" s="109"/>
-      <c r="K21" s="109"/>
-      <c r="L21" s="110"/>
-      <c r="M21" s="109"/>
-      <c r="N21" s="111"/>
-      <c r="O21" s="110"/>
-      <c r="P21" s="110"/>
-      <c r="Q21" s="110"/>
-      <c r="R21" s="110"/>
+      <c r="I21" s="124"/>
+      <c r="J21" s="124"/>
+      <c r="K21" s="124"/>
+      <c r="L21" s="123"/>
+      <c r="M21" s="124"/>
+      <c r="N21" s="125"/>
+      <c r="O21" s="123"/>
+      <c r="P21" s="123"/>
+      <c r="Q21" s="123"/>
+      <c r="R21" s="123"/>
     </row>
     <row r="22" spans="1:18" ht="15" customHeight="1">
-      <c r="A22" s="119"/>
+      <c r="A22" s="111"/>
       <c r="B22" s="27" t="s">
         <v>164</v>
       </c>
@@ -3130,57 +3145,57 @@
       </c>
       <c r="E22" s="28"/>
       <c r="F22" s="8"/>
-      <c r="I22" s="109" t="s">
+      <c r="I22" s="124" t="s">
         <v>177</v>
       </c>
-      <c r="J22" s="109">
+      <c r="J22" s="124">
         <v>3</v>
       </c>
-      <c r="K22" s="109">
+      <c r="K22" s="124">
         <v>6</v>
       </c>
-      <c r="L22" s="110" t="s">
+      <c r="L22" s="123" t="s">
         <v>178</v>
       </c>
-      <c r="M22" s="109" t="s">
+      <c r="M22" s="124" t="s">
         <v>26</v>
       </c>
-      <c r="N22" s="111" t="s">
+      <c r="N22" s="125" t="s">
         <v>37</v>
       </c>
-      <c r="O22" s="110" t="s">
+      <c r="O22" s="123" t="s">
         <v>179</v>
       </c>
-      <c r="P22" s="110" t="s">
+      <c r="P22" s="123" t="s">
         <v>180</v>
       </c>
-      <c r="Q22" s="110" t="s">
+      <c r="Q22" s="123" t="s">
         <v>181</v>
       </c>
-      <c r="R22" s="110" t="s">
+      <c r="R22" s="123" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="15" customHeight="1">
-      <c r="A23" s="119"/>
+      <c r="A23" s="111"/>
       <c r="B23" s="27"/>
       <c r="C23" s="28"/>
       <c r="D23" s="28"/>
       <c r="E23" s="28"/>
       <c r="F23" s="8"/>
-      <c r="I23" s="109"/>
-      <c r="J23" s="109"/>
-      <c r="K23" s="109"/>
-      <c r="L23" s="110"/>
-      <c r="M23" s="109"/>
-      <c r="N23" s="111"/>
-      <c r="O23" s="110"/>
-      <c r="P23" s="110"/>
-      <c r="Q23" s="110"/>
-      <c r="R23" s="110"/>
+      <c r="I23" s="124"/>
+      <c r="J23" s="124"/>
+      <c r="K23" s="124"/>
+      <c r="L23" s="123"/>
+      <c r="M23" s="124"/>
+      <c r="N23" s="125"/>
+      <c r="O23" s="123"/>
+      <c r="P23" s="123"/>
+      <c r="Q23" s="123"/>
+      <c r="R23" s="123"/>
     </row>
     <row r="24" spans="1:18" ht="15" customHeight="1">
-      <c r="A24" s="119"/>
+      <c r="A24" s="111"/>
       <c r="B24" s="27"/>
       <c r="C24" s="28"/>
       <c r="D24" s="28"/>
@@ -3188,7 +3203,7 @@
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:18" ht="15" customHeight="1">
-      <c r="A25" s="119"/>
+      <c r="A25" s="111"/>
       <c r="B25" s="27"/>
       <c r="C25" s="28"/>
       <c r="D25" s="28"/>
@@ -3413,49 +3428,16 @@
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="A10:A17"/>
-    <mergeCell ref="A18:A25"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="R16:R17"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="O14:O15"/>
-    <mergeCell ref="P14:P15"/>
-    <mergeCell ref="Q14:Q15"/>
-    <mergeCell ref="R14:R15"/>
-    <mergeCell ref="P16:P17"/>
-    <mergeCell ref="Q16:Q17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="O12:O13"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="Q12:Q13"/>
-    <mergeCell ref="R12:R13"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="O20:O21"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="I18:I19"/>
     <mergeCell ref="M22:M23"/>
     <mergeCell ref="R18:R19"/>
     <mergeCell ref="Q20:Q21"/>
@@ -3472,16 +3454,49 @@
     <mergeCell ref="M18:M19"/>
     <mergeCell ref="M20:M21"/>
     <mergeCell ref="N18:N19"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="O20:O21"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="O12:O13"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="Q12:Q13"/>
+    <mergeCell ref="R12:R13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="R16:R17"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="O14:O15"/>
+    <mergeCell ref="P14:P15"/>
+    <mergeCell ref="Q14:Q15"/>
+    <mergeCell ref="R14:R15"/>
+    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="Q16:Q17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3492,7 +3507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B769BC50-9623-4726-8971-E5FD68E08F76}">
   <dimension ref="A1:T88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
@@ -3518,16 +3533,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="17.25">
-      <c r="A1" s="148"/>
-      <c r="B1" s="149"/>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
-      <c r="H1" s="149"/>
-      <c r="I1" s="149"/>
-      <c r="J1" s="149"/>
+      <c r="A1" s="135"/>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="136"/>
+      <c r="J1" s="136"/>
     </row>
     <row r="2" spans="1:20" ht="33">
       <c r="A2" s="67" t="s">
@@ -3548,14 +3563,14 @@
       <c r="F2" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="145" t="s">
+      <c r="G2" s="144" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="145"/>
-      <c r="I2" s="145" t="s">
+      <c r="H2" s="144"/>
+      <c r="I2" s="144" t="s">
         <v>111</v>
       </c>
-      <c r="J2" s="145"/>
+      <c r="J2" s="144"/>
       <c r="L2" s="2" t="s">
         <v>16</v>
       </c>
@@ -3582,7 +3597,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="30">
-      <c r="A3" s="146" t="s">
+      <c r="A3" s="145" t="s">
         <v>112</v>
       </c>
       <c r="B3" s="9"/>
@@ -3596,10 +3611,10 @@
         <v>142</v>
       </c>
       <c r="F3" s="9"/>
-      <c r="G3" s="147"/>
-      <c r="H3" s="147"/>
-      <c r="I3" s="147"/>
-      <c r="J3" s="147"/>
+      <c r="G3" s="146"/>
+      <c r="H3" s="146"/>
+      <c r="I3" s="146"/>
+      <c r="J3" s="146"/>
       <c r="L3" s="3" t="s">
         <v>216</v>
       </c>
@@ -3624,12 +3639,12 @@
       <c r="S3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="T3" s="164" t="s">
-        <v>308</v>
+      <c r="T3" s="109" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="18.75" customHeight="1">
-      <c r="A4" s="146"/>
+      <c r="A4" s="145"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
         <v>96</v>
@@ -3641,10 +3656,10 @@
         <v>142</v>
       </c>
       <c r="F4" s="9"/>
-      <c r="G4" s="147"/>
-      <c r="H4" s="147"/>
-      <c r="I4" s="147"/>
-      <c r="J4" s="147"/>
+      <c r="G4" s="146"/>
+      <c r="H4" s="146"/>
+      <c r="I4" s="146"/>
+      <c r="J4" s="146"/>
       <c r="L4" s="3" t="s">
         <v>217</v>
       </c>
@@ -3669,12 +3684,12 @@
       <c r="S4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="T4" s="164" t="s">
-        <v>308</v>
+      <c r="T4" s="109" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="27" customHeight="1">
-      <c r="A5" s="146"/>
+      <c r="A5" s="145"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9" t="s">
         <v>97</v>
@@ -3686,12 +3701,12 @@
         <v>142</v>
       </c>
       <c r="F5" s="9"/>
-      <c r="G5" s="147"/>
-      <c r="H5" s="147"/>
-      <c r="I5" s="147"/>
-      <c r="J5" s="147"/>
+      <c r="G5" s="146"/>
+      <c r="H5" s="146"/>
+      <c r="I5" s="146"/>
+      <c r="J5" s="146"/>
       <c r="L5" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="M5" s="4">
         <v>40</v>
@@ -3714,20 +3729,20 @@
       <c r="S5" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="T5" s="164" t="s">
-        <v>308</v>
+      <c r="T5" s="109" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="17.25">
-      <c r="A6" s="140" t="s">
-        <v>286</v>
+      <c r="A6" s="147" t="s">
+        <v>285</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10" t="s">
         <v>97</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>142</v>
@@ -3735,12 +3750,12 @@
       <c r="F6" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="G6" s="141"/>
-      <c r="H6" s="141"/>
-      <c r="I6" s="141"/>
-      <c r="J6" s="141"/>
+      <c r="G6" s="150"/>
+      <c r="H6" s="150"/>
+      <c r="I6" s="150"/>
+      <c r="J6" s="150"/>
       <c r="L6" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M6" s="4">
         <v>2</v>
@@ -3764,11 +3779,11 @@
         <v>234</v>
       </c>
       <c r="T6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="19.5" customHeight="1">
-      <c r="A7" s="140"/>
+      <c r="A7" s="147"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10" t="s">
         <v>98</v>
@@ -3811,17 +3826,17 @@
         <v>237</v>
       </c>
       <c r="T7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="18.75" customHeight="1">
-      <c r="A8" s="140"/>
+      <c r="A8" s="147"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10" t="s">
         <v>183</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>142</v>
@@ -3843,7 +3858,7 @@
         <v>2</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="P8" s="4" t="s">
         <v>141</v>
@@ -3858,7 +3873,7 @@
         <v>239</v>
       </c>
       <c r="T8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="16.5" customHeight="1">
@@ -3908,10 +3923,10 @@
       <c r="F10" s="72" t="s">
         <v>240</v>
       </c>
-      <c r="G10" s="144"/>
-      <c r="H10" s="144"/>
-      <c r="I10" s="144"/>
-      <c r="J10" s="144"/>
+      <c r="G10" s="143"/>
+      <c r="H10" s="143"/>
+      <c r="I10" s="143"/>
+      <c r="J10" s="143"/>
       <c r="L10" s="3"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
@@ -3930,7 +3945,7 @@
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>25</v>
@@ -3938,10 +3953,10 @@
       <c r="F11" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="G11" s="143"/>
-      <c r="H11" s="143"/>
-      <c r="I11" s="143"/>
-      <c r="J11" s="143"/>
+      <c r="G11" s="148"/>
+      <c r="H11" s="148"/>
+      <c r="I11" s="148"/>
+      <c r="J11" s="148"/>
       <c r="S11" s="4"/>
     </row>
     <row r="12" spans="1:20" ht="17.25">
@@ -4066,14 +4081,14 @@
     </row>
     <row r="16" spans="1:20" ht="17.25">
       <c r="A16" s="74" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B16" s="74" t="s">
         <v>120</v>
       </c>
       <c r="C16" s="74"/>
       <c r="D16" s="74" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E16" s="74" t="s">
         <v>25</v>
@@ -4169,23 +4184,23 @@
       <c r="F19" s="78" t="s">
         <v>240</v>
       </c>
-      <c r="G19" s="139"/>
-      <c r="H19" s="139"/>
-      <c r="I19" s="139"/>
-      <c r="J19" s="139"/>
+      <c r="G19" s="151"/>
+      <c r="H19" s="151"/>
+      <c r="I19" s="151"/>
+      <c r="J19" s="151"/>
     </row>
     <row r="20" spans="1:19" ht="18" thickBot="1">
       <c r="A20" s="80" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B20" s="81" t="s">
         <v>121</v>
       </c>
       <c r="C20" s="82" t="s">
+        <v>292</v>
+      </c>
+      <c r="D20" s="81" t="s">
         <v>293</v>
-      </c>
-      <c r="D20" s="81" t="s">
-        <v>294</v>
       </c>
       <c r="E20" s="81" t="s">
         <v>25</v>
@@ -4193,10 +4208,10 @@
       <c r="F20" s="82" t="s">
         <v>240</v>
       </c>
-      <c r="G20" s="134"/>
-      <c r="H20" s="134"/>
-      <c r="I20" s="134"/>
-      <c r="J20" s="134"/>
+      <c r="G20" s="137"/>
+      <c r="H20" s="137"/>
+      <c r="I20" s="137"/>
+      <c r="J20" s="137"/>
     </row>
     <row r="21" spans="1:19" ht="17.25">
       <c r="A21" s="83" t="s">
@@ -4215,17 +4230,17 @@
         <v>222</v>
       </c>
       <c r="F21" s="85"/>
-      <c r="G21" s="135"/>
-      <c r="H21" s="135"/>
-      <c r="I21" s="135"/>
-      <c r="J21" s="136"/>
+      <c r="G21" s="139"/>
+      <c r="H21" s="139"/>
+      <c r="I21" s="139"/>
+      <c r="J21" s="140"/>
     </row>
     <row r="22" spans="1:19" ht="17.25">
       <c r="A22" s="86">
         <v>11</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>137</v>
@@ -4237,17 +4252,17 @@
         <v>224</v>
       </c>
       <c r="F22" s="1"/>
-      <c r="G22" s="137"/>
-      <c r="H22" s="137"/>
-      <c r="I22" s="137"/>
-      <c r="J22" s="138"/>
+      <c r="G22" s="132"/>
+      <c r="H22" s="132"/>
+      <c r="I22" s="132"/>
+      <c r="J22" s="141"/>
     </row>
     <row r="23" spans="1:19" ht="17.25">
       <c r="A23" s="86">
         <v>12</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>229</v>
@@ -4259,10 +4274,10 @@
         <v>225</v>
       </c>
       <c r="F23" s="1"/>
-      <c r="G23" s="137"/>
-      <c r="H23" s="137"/>
-      <c r="I23" s="137"/>
-      <c r="J23" s="138"/>
+      <c r="G23" s="132"/>
+      <c r="H23" s="132"/>
+      <c r="I23" s="132"/>
+      <c r="J23" s="141"/>
     </row>
     <row r="24" spans="1:19" ht="18" thickBot="1">
       <c r="A24" s="87">
@@ -4277,14 +4292,14 @@
       <c r="D24" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="131" t="s">
+      <c r="E24" s="134" t="s">
         <v>228</v>
       </c>
-      <c r="F24" s="131"/>
-      <c r="G24" s="132"/>
-      <c r="H24" s="132"/>
-      <c r="I24" s="132"/>
-      <c r="J24" s="133"/>
+      <c r="F24" s="134"/>
+      <c r="G24" s="138"/>
+      <c r="H24" s="138"/>
+      <c r="I24" s="138"/>
+      <c r="J24" s="149"/>
     </row>
     <row r="25" spans="1:19" ht="17.25">
       <c r="A25" s="93"/>
@@ -4293,10 +4308,10 @@
       <c r="D25" s="91"/>
       <c r="E25" s="91"/>
       <c r="F25" s="34"/>
-      <c r="G25" s="137"/>
-      <c r="H25" s="137"/>
-      <c r="I25" s="137"/>
-      <c r="J25" s="137"/>
+      <c r="G25" s="132"/>
+      <c r="H25" s="132"/>
+      <c r="I25" s="132"/>
+      <c r="J25" s="132"/>
     </row>
     <row r="26" spans="1:19" ht="18" thickBot="1">
       <c r="A26" s="94"/>
@@ -4305,10 +4320,10 @@
       <c r="D26" s="91"/>
       <c r="E26" s="91"/>
       <c r="F26" s="34"/>
-      <c r="G26" s="137"/>
-      <c r="H26" s="137"/>
-      <c r="I26" s="137"/>
-      <c r="J26" s="137"/>
+      <c r="G26" s="132"/>
+      <c r="H26" s="132"/>
+      <c r="I26" s="132"/>
+      <c r="J26" s="132"/>
     </row>
     <row r="27" spans="1:19" ht="16.5" customHeight="1" thickBot="1">
       <c r="A27" s="95"/>
@@ -4317,10 +4332,10 @@
       <c r="D27" s="34"/>
       <c r="E27" s="34"/>
       <c r="F27" s="34"/>
-      <c r="G27" s="137"/>
-      <c r="H27" s="137"/>
-      <c r="I27" s="137"/>
-      <c r="J27" s="137"/>
+      <c r="G27" s="132"/>
+      <c r="H27" s="132"/>
+      <c r="I27" s="132"/>
+      <c r="J27" s="132"/>
     </row>
     <row r="28" spans="1:19" ht="16.5" customHeight="1" thickBot="1">
       <c r="A28" s="96"/>
@@ -4329,10 +4344,10 @@
       <c r="D28" s="34"/>
       <c r="E28" s="34"/>
       <c r="F28" s="34"/>
-      <c r="G28" s="137"/>
-      <c r="H28" s="137"/>
-      <c r="I28" s="137"/>
-      <c r="J28" s="137"/>
+      <c r="G28" s="132"/>
+      <c r="H28" s="132"/>
+      <c r="I28" s="132"/>
+      <c r="J28" s="132"/>
     </row>
     <row r="29" spans="1:19" ht="14.25" customHeight="1" thickBot="1">
       <c r="A29" s="96"/>
@@ -4341,10 +4356,10 @@
       <c r="D29" s="34"/>
       <c r="E29" s="34"/>
       <c r="F29" s="34"/>
-      <c r="G29" s="137"/>
-      <c r="H29" s="137"/>
-      <c r="I29" s="137"/>
-      <c r="J29" s="137"/>
+      <c r="G29" s="132"/>
+      <c r="H29" s="132"/>
+      <c r="I29" s="132"/>
+      <c r="J29" s="132"/>
     </row>
     <row r="30" spans="1:19" ht="17.25">
       <c r="A30" s="96"/>
@@ -4353,10 +4368,10 @@
       <c r="D30" s="34"/>
       <c r="E30" s="34"/>
       <c r="F30" s="34"/>
-      <c r="G30" s="137"/>
-      <c r="H30" s="137"/>
-      <c r="I30" s="137"/>
-      <c r="J30" s="137"/>
+      <c r="G30" s="132"/>
+      <c r="H30" s="132"/>
+      <c r="I30" s="132"/>
+      <c r="J30" s="132"/>
     </row>
     <row r="31" spans="1:19" ht="17.25">
       <c r="A31" s="96"/>
@@ -4365,10 +4380,10 @@
       <c r="D31" s="34"/>
       <c r="E31" s="34"/>
       <c r="F31" s="34"/>
-      <c r="G31" s="137"/>
-      <c r="H31" s="137"/>
-      <c r="I31" s="137"/>
-      <c r="J31" s="137"/>
+      <c r="G31" s="132"/>
+      <c r="H31" s="132"/>
+      <c r="I31" s="132"/>
+      <c r="J31" s="132"/>
     </row>
     <row r="32" spans="1:19" ht="17.25">
       <c r="A32" s="96"/>
@@ -4377,10 +4392,10 @@
       <c r="D32" s="34"/>
       <c r="E32" s="34"/>
       <c r="F32" s="34"/>
-      <c r="G32" s="137"/>
-      <c r="H32" s="137"/>
-      <c r="I32" s="137"/>
-      <c r="J32" s="137"/>
+      <c r="G32" s="132"/>
+      <c r="H32" s="132"/>
+      <c r="I32" s="132"/>
+      <c r="J32" s="132"/>
     </row>
     <row r="33" spans="1:10" ht="18" thickBot="1">
       <c r="A33" s="96"/>
@@ -4389,10 +4404,10 @@
       <c r="D33" s="34"/>
       <c r="E33" s="34"/>
       <c r="F33" s="34"/>
-      <c r="G33" s="137"/>
-      <c r="H33" s="137"/>
-      <c r="I33" s="137"/>
-      <c r="J33" s="137"/>
+      <c r="G33" s="132"/>
+      <c r="H33" s="132"/>
+      <c r="I33" s="132"/>
+      <c r="J33" s="132"/>
     </row>
     <row r="34" spans="1:10" ht="18" thickBot="1">
       <c r="A34" s="96"/>
@@ -4401,10 +4416,10 @@
       <c r="D34" s="34"/>
       <c r="E34" s="34"/>
       <c r="F34" s="34"/>
-      <c r="G34" s="137"/>
-      <c r="H34" s="137"/>
-      <c r="I34" s="137"/>
-      <c r="J34" s="137"/>
+      <c r="G34" s="132"/>
+      <c r="H34" s="132"/>
+      <c r="I34" s="132"/>
+      <c r="J34" s="132"/>
     </row>
     <row r="35" spans="1:10" ht="17.25">
       <c r="A35" s="97"/>
@@ -4413,10 +4428,10 @@
       <c r="D35" s="34"/>
       <c r="E35" s="34"/>
       <c r="F35" s="34"/>
-      <c r="G35" s="137"/>
-      <c r="H35" s="137"/>
-      <c r="I35" s="137"/>
-      <c r="J35" s="137"/>
+      <c r="G35" s="132"/>
+      <c r="H35" s="132"/>
+      <c r="I35" s="132"/>
+      <c r="J35" s="132"/>
     </row>
     <row r="36" spans="1:10" ht="18" thickBot="1">
       <c r="A36" s="98"/>
@@ -4425,10 +4440,10 @@
       <c r="D36" s="34"/>
       <c r="E36" s="34"/>
       <c r="F36" s="34"/>
-      <c r="G36" s="137"/>
-      <c r="H36" s="137"/>
-      <c r="I36" s="137"/>
-      <c r="J36" s="137"/>
+      <c r="G36" s="132"/>
+      <c r="H36" s="132"/>
+      <c r="I36" s="132"/>
+      <c r="J36" s="132"/>
     </row>
     <row r="37" spans="1:10" ht="17.25">
       <c r="A37" s="99"/>
@@ -4437,10 +4452,10 @@
       <c r="D37" s="34"/>
       <c r="E37" s="34"/>
       <c r="F37" s="34"/>
-      <c r="G37" s="137"/>
-      <c r="H37" s="137"/>
-      <c r="I37" s="137"/>
-      <c r="J37" s="137"/>
+      <c r="G37" s="132"/>
+      <c r="H37" s="132"/>
+      <c r="I37" s="132"/>
+      <c r="J37" s="132"/>
     </row>
     <row r="38" spans="1:10" ht="17.25">
       <c r="A38" s="34"/>
@@ -4449,10 +4464,10 @@
       <c r="D38" s="34"/>
       <c r="E38" s="34"/>
       <c r="F38" s="34"/>
-      <c r="G38" s="137"/>
-      <c r="H38" s="137"/>
-      <c r="I38" s="137"/>
-      <c r="J38" s="137"/>
+      <c r="G38" s="132"/>
+      <c r="H38" s="132"/>
+      <c r="I38" s="132"/>
+      <c r="J38" s="132"/>
     </row>
     <row r="39" spans="1:10" ht="17.25">
       <c r="A39" s="34"/>
@@ -4461,10 +4476,10 @@
       <c r="D39" s="34"/>
       <c r="E39" s="34"/>
       <c r="F39" s="34"/>
-      <c r="G39" s="137"/>
-      <c r="H39" s="137"/>
-      <c r="I39" s="137"/>
-      <c r="J39" s="137"/>
+      <c r="G39" s="132"/>
+      <c r="H39" s="132"/>
+      <c r="I39" s="132"/>
+      <c r="J39" s="132"/>
     </row>
     <row r="40" spans="1:10" ht="17.25">
       <c r="A40" s="34"/>
@@ -4473,10 +4488,10 @@
       <c r="D40" s="34"/>
       <c r="E40" s="34"/>
       <c r="F40" s="34"/>
-      <c r="G40" s="137"/>
-      <c r="H40" s="137"/>
-      <c r="I40" s="137"/>
-      <c r="J40" s="137"/>
+      <c r="G40" s="132"/>
+      <c r="H40" s="132"/>
+      <c r="I40" s="132"/>
+      <c r="J40" s="132"/>
     </row>
     <row r="41" spans="1:10" ht="17.25">
       <c r="A41" s="101"/>
@@ -4485,10 +4500,10 @@
       <c r="D41" s="34"/>
       <c r="E41" s="34"/>
       <c r="F41" s="34"/>
-      <c r="G41" s="137"/>
-      <c r="H41" s="137"/>
-      <c r="I41" s="137"/>
-      <c r="J41" s="137"/>
+      <c r="G41" s="132"/>
+      <c r="H41" s="132"/>
+      <c r="I41" s="132"/>
+      <c r="J41" s="132"/>
     </row>
     <row r="42" spans="1:10" ht="17.25">
       <c r="A42" s="102"/>
@@ -4497,10 +4512,10 @@
       <c r="D42" s="34"/>
       <c r="E42" s="34"/>
       <c r="F42" s="34"/>
-      <c r="G42" s="137"/>
-      <c r="H42" s="137"/>
-      <c r="I42" s="137"/>
-      <c r="J42" s="137"/>
+      <c r="G42" s="132"/>
+      <c r="H42" s="132"/>
+      <c r="I42" s="132"/>
+      <c r="J42" s="132"/>
     </row>
     <row r="43" spans="1:10" ht="17.25">
       <c r="A43" s="104"/>
@@ -4509,10 +4524,10 @@
       <c r="D43" s="34"/>
       <c r="E43" s="34"/>
       <c r="F43" s="34"/>
-      <c r="G43" s="137"/>
-      <c r="H43" s="137"/>
-      <c r="I43" s="137"/>
-      <c r="J43" s="137"/>
+      <c r="G43" s="132"/>
+      <c r="H43" s="132"/>
+      <c r="I43" s="132"/>
+      <c r="J43" s="132"/>
     </row>
     <row r="44" spans="1:10" ht="17.25">
       <c r="A44" s="105"/>
@@ -4521,10 +4536,10 @@
       <c r="D44" s="34"/>
       <c r="E44" s="34"/>
       <c r="F44" s="34"/>
-      <c r="G44" s="137"/>
-      <c r="H44" s="137"/>
-      <c r="I44" s="137"/>
-      <c r="J44" s="137"/>
+      <c r="G44" s="132"/>
+      <c r="H44" s="132"/>
+      <c r="I44" s="132"/>
+      <c r="J44" s="132"/>
     </row>
     <row r="45" spans="1:10" ht="17.25">
       <c r="A45" s="34"/>
@@ -4609,8 +4624,8 @@
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
-      <c r="E55" s="150"/>
-      <c r="F55" s="150"/>
+      <c r="E55" s="133"/>
+      <c r="F55" s="133"/>
     </row>
     <row r="57" spans="1:10" ht="17.25">
       <c r="E57" s="37"/>
@@ -4640,14 +4655,14 @@
       <c r="F66" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="G66" s="145" t="s">
+      <c r="G66" s="144" t="s">
         <v>5</v>
       </c>
-      <c r="H66" s="145"/>
-      <c r="I66" s="145" t="s">
+      <c r="H66" s="144"/>
+      <c r="I66" s="144" t="s">
         <v>111</v>
       </c>
-      <c r="J66" s="145"/>
+      <c r="J66" s="144"/>
       <c r="L66" s="2" t="s">
         <v>16</v>
       </c>
@@ -4674,7 +4689,7 @@
       </c>
     </row>
     <row r="67" spans="1:19" ht="17.25">
-      <c r="A67" s="146" t="s">
+      <c r="A67" s="145" t="s">
         <v>112</v>
       </c>
       <c r="B67" s="9"/>
@@ -4688,10 +4703,10 @@
         <v>142</v>
       </c>
       <c r="F67" s="9"/>
-      <c r="G67" s="147"/>
-      <c r="H67" s="147"/>
-      <c r="I67" s="147"/>
-      <c r="J67" s="147"/>
+      <c r="G67" s="146"/>
+      <c r="H67" s="146"/>
+      <c r="I67" s="146"/>
+      <c r="J67" s="146"/>
       <c r="L67" s="3" t="s">
         <v>216</v>
       </c>
@@ -4718,7 +4733,7 @@
       </c>
     </row>
     <row r="68" spans="1:19" ht="17.25">
-      <c r="A68" s="146"/>
+      <c r="A68" s="145"/>
       <c r="B68" s="9"/>
       <c r="C68" s="9" t="s">
         <v>96</v>
@@ -4730,10 +4745,10 @@
         <v>142</v>
       </c>
       <c r="F68" s="9"/>
-      <c r="G68" s="147"/>
-      <c r="H68" s="147"/>
-      <c r="I68" s="147"/>
-      <c r="J68" s="147"/>
+      <c r="G68" s="146"/>
+      <c r="H68" s="146"/>
+      <c r="I68" s="146"/>
+      <c r="J68" s="146"/>
       <c r="L68" s="3" t="s">
         <v>217</v>
       </c>
@@ -4760,7 +4775,7 @@
       </c>
     </row>
     <row r="69" spans="1:19" ht="17.25">
-      <c r="A69" s="146"/>
+      <c r="A69" s="145"/>
       <c r="B69" s="9"/>
       <c r="C69" s="9" t="s">
         <v>97</v>
@@ -4772,12 +4787,12 @@
         <v>142</v>
       </c>
       <c r="F69" s="9"/>
-      <c r="G69" s="147"/>
-      <c r="H69" s="147"/>
-      <c r="I69" s="147"/>
-      <c r="J69" s="147"/>
+      <c r="G69" s="146"/>
+      <c r="H69" s="146"/>
+      <c r="I69" s="146"/>
+      <c r="J69" s="146"/>
       <c r="L69" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="M69" s="4">
         <v>40</v>
@@ -4802,15 +4817,15 @@
       </c>
     </row>
     <row r="70" spans="1:19" ht="17.25">
-      <c r="A70" s="140" t="s">
-        <v>286</v>
+      <c r="A70" s="147" t="s">
+        <v>285</v>
       </c>
       <c r="B70" s="10"/>
       <c r="C70" s="10" t="s">
         <v>97</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E70" s="10" t="s">
         <v>142</v>
@@ -4818,12 +4833,12 @@
       <c r="F70" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="G70" s="141"/>
-      <c r="H70" s="141"/>
-      <c r="I70" s="141"/>
-      <c r="J70" s="141"/>
+      <c r="G70" s="150"/>
+      <c r="H70" s="150"/>
+      <c r="I70" s="150"/>
+      <c r="J70" s="150"/>
       <c r="L70" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M70" s="4">
         <v>2</v>
@@ -4848,7 +4863,7 @@
       </c>
     </row>
     <row r="71" spans="1:19" ht="17.25">
-      <c r="A71" s="140"/>
+      <c r="A71" s="147"/>
       <c r="B71" s="10"/>
       <c r="C71" s="10" t="s">
         <v>98</v>
@@ -4892,13 +4907,13 @@
       </c>
     </row>
     <row r="72" spans="1:19" ht="17.25">
-      <c r="A72" s="140"/>
+      <c r="A72" s="147"/>
       <c r="B72" s="10"/>
       <c r="C72" s="10" t="s">
         <v>183</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E72" s="10" t="s">
         <v>142</v>
@@ -4920,7 +4935,7 @@
         <v>2</v>
       </c>
       <c r="O72" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="P72" s="4" t="s">
         <v>141</v>
@@ -4982,10 +4997,10 @@
       <c r="F74" s="72" t="s">
         <v>240</v>
       </c>
-      <c r="G74" s="144"/>
-      <c r="H74" s="144"/>
-      <c r="I74" s="144"/>
-      <c r="J74" s="144"/>
+      <c r="G74" s="143"/>
+      <c r="H74" s="143"/>
+      <c r="I74" s="143"/>
+      <c r="J74" s="143"/>
       <c r="L74" s="3"/>
       <c r="M74" s="4"/>
       <c r="N74" s="4"/>
@@ -5004,7 +5019,7 @@
       </c>
       <c r="C75" s="11"/>
       <c r="D75" s="11" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E75" s="11" t="s">
         <v>25</v>
@@ -5012,10 +5027,10 @@
       <c r="F75" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="G75" s="143"/>
-      <c r="H75" s="143"/>
-      <c r="I75" s="143"/>
-      <c r="J75" s="143"/>
+      <c r="G75" s="148"/>
+      <c r="H75" s="148"/>
+      <c r="I75" s="148"/>
+      <c r="J75" s="148"/>
       <c r="S75" s="4"/>
     </row>
     <row r="76" spans="1:19" ht="17.25">
@@ -5140,14 +5155,14 @@
     </row>
     <row r="80" spans="1:19" ht="17.25">
       <c r="A80" s="74" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B80" s="74" t="s">
         <v>120</v>
       </c>
       <c r="C80" s="74"/>
       <c r="D80" s="74" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E80" s="74" t="s">
         <v>25</v>
@@ -5243,23 +5258,23 @@
       <c r="F83" s="78" t="s">
         <v>240</v>
       </c>
-      <c r="G83" s="139"/>
-      <c r="H83" s="139"/>
-      <c r="I83" s="139"/>
-      <c r="J83" s="139"/>
+      <c r="G83" s="151"/>
+      <c r="H83" s="151"/>
+      <c r="I83" s="151"/>
+      <c r="J83" s="151"/>
     </row>
     <row r="84" spans="1:19" ht="18" thickBot="1">
       <c r="A84" s="80" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B84" s="81" t="s">
         <v>121</v>
       </c>
       <c r="C84" s="82" t="s">
+        <v>292</v>
+      </c>
+      <c r="D84" s="81" t="s">
         <v>293</v>
-      </c>
-      <c r="D84" s="81" t="s">
-        <v>294</v>
       </c>
       <c r="E84" s="81" t="s">
         <v>25</v>
@@ -5267,10 +5282,10 @@
       <c r="F84" s="82" t="s">
         <v>240</v>
       </c>
-      <c r="G84" s="134"/>
-      <c r="H84" s="134"/>
-      <c r="I84" s="134"/>
-      <c r="J84" s="134"/>
+      <c r="G84" s="137"/>
+      <c r="H84" s="137"/>
+      <c r="I84" s="137"/>
+      <c r="J84" s="137"/>
     </row>
     <row r="85" spans="1:19" ht="17.25">
       <c r="A85" s="83" t="s">
@@ -5289,17 +5304,17 @@
         <v>222</v>
       </c>
       <c r="F85" s="85"/>
-      <c r="G85" s="135"/>
-      <c r="H85" s="135"/>
-      <c r="I85" s="135"/>
-      <c r="J85" s="136"/>
+      <c r="G85" s="139"/>
+      <c r="H85" s="139"/>
+      <c r="I85" s="139"/>
+      <c r="J85" s="140"/>
     </row>
     <row r="86" spans="1:19" ht="17.25">
       <c r="A86" s="86">
         <v>11</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>137</v>
@@ -5311,17 +5326,17 @@
         <v>224</v>
       </c>
       <c r="F86" s="1"/>
-      <c r="G86" s="137"/>
-      <c r="H86" s="137"/>
-      <c r="I86" s="137"/>
-      <c r="J86" s="138"/>
+      <c r="G86" s="132"/>
+      <c r="H86" s="132"/>
+      <c r="I86" s="132"/>
+      <c r="J86" s="141"/>
     </row>
     <row r="87" spans="1:19" ht="17.25">
       <c r="A87" s="86">
         <v>12</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>229</v>
@@ -5333,10 +5348,10 @@
         <v>225</v>
       </c>
       <c r="F87" s="1"/>
-      <c r="G87" s="137"/>
-      <c r="H87" s="137"/>
-      <c r="I87" s="137"/>
-      <c r="J87" s="138"/>
+      <c r="G87" s="132"/>
+      <c r="H87" s="132"/>
+      <c r="I87" s="132"/>
+      <c r="J87" s="141"/>
     </row>
     <row r="88" spans="1:19" ht="18" thickBot="1">
       <c r="A88" s="87">
@@ -5351,37 +5366,75 @@
       <c r="D88" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="E88" s="131" t="s">
+      <c r="E88" s="134" t="s">
         <v>228</v>
       </c>
-      <c r="F88" s="131"/>
-      <c r="G88" s="132"/>
-      <c r="H88" s="132"/>
-      <c r="I88" s="132"/>
-      <c r="J88" s="133"/>
+      <c r="F88" s="134"/>
+      <c r="G88" s="138"/>
+      <c r="H88" s="138"/>
+      <c r="I88" s="138"/>
+      <c r="J88" s="149"/>
     </row>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="E88:F88"/>
+    <mergeCell ref="G88:H88"/>
+    <mergeCell ref="I88:J88"/>
+    <mergeCell ref="G84:H84"/>
+    <mergeCell ref="I84:J84"/>
+    <mergeCell ref="G85:H85"/>
+    <mergeCell ref="I85:J85"/>
+    <mergeCell ref="G86:H86"/>
+    <mergeCell ref="I86:J86"/>
+    <mergeCell ref="G83:H83"/>
+    <mergeCell ref="I83:J83"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="G70:H70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="G87:H87"/>
+    <mergeCell ref="I87:J87"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="I74:J74"/>
+    <mergeCell ref="G75:H75"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="I67:J67"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="I68:J68"/>
+    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="I69:J69"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="G10:H10"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="G36:H36"/>
     <mergeCell ref="I36:J36"/>
@@ -5406,66 +5459,28 @@
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="G31:H31"/>
     <mergeCell ref="I30:J30"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
     <mergeCell ref="G34:H34"/>
     <mergeCell ref="I34:J34"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="G74:H74"/>
-    <mergeCell ref="I74:J74"/>
-    <mergeCell ref="G75:H75"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="A67:A69"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="I67:J67"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="I68:J68"/>
-    <mergeCell ref="G69:H69"/>
-    <mergeCell ref="I69:J69"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="G83:H83"/>
-    <mergeCell ref="I83:J83"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="G70:H70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="G73:H73"/>
-    <mergeCell ref="I73:J73"/>
-    <mergeCell ref="G87:H87"/>
-    <mergeCell ref="I87:J87"/>
-    <mergeCell ref="E88:F88"/>
-    <mergeCell ref="G88:H88"/>
-    <mergeCell ref="I88:J88"/>
-    <mergeCell ref="G84:H84"/>
-    <mergeCell ref="I84:J84"/>
-    <mergeCell ref="G85:H85"/>
-    <mergeCell ref="I85:J85"/>
-    <mergeCell ref="G86:H86"/>
-    <mergeCell ref="I86:J86"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5477,8 +5492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27F8DC3-BDE0-43F3-979D-2CCDC5541D2C}">
   <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -5502,14 +5517,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="155" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="160"/>
+      <c r="B1" s="156"/>
+      <c r="C1" s="156"/>
+      <c r="D1" s="156"/>
+      <c r="E1" s="156"/>
+      <c r="F1" s="156"/>
     </row>
     <row r="2" spans="1:20" ht="15" customHeight="1">
       <c r="A2" s="42" t="s">
@@ -5530,17 +5545,17 @@
       <c r="F2" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="161" t="s">
+      <c r="G2" s="157" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="161"/>
-      <c r="I2" s="161" t="s">
+      <c r="H2" s="157"/>
+      <c r="I2" s="157" t="s">
         <v>111</v>
       </c>
-      <c r="J2" s="161"/>
+      <c r="J2" s="157"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A3" s="162" t="s">
+      <c r="A3" s="152" t="s">
         <v>81</v>
       </c>
       <c r="B3" s="43"/>
@@ -5554,10 +5569,10 @@
         <v>142</v>
       </c>
       <c r="F3" s="43"/>
-      <c r="G3" s="151"/>
-      <c r="H3" s="152"/>
-      <c r="I3" s="151"/>
-      <c r="J3" s="152"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="154"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="154"/>
       <c r="L3" s="41" t="s">
         <v>58</v>
       </c>
@@ -5570,7 +5585,7 @@
       <c r="S3" s="46"/>
     </row>
     <row r="4" spans="1:20" ht="30" customHeight="1">
-      <c r="A4" s="162"/>
+      <c r="A4" s="152"/>
       <c r="B4" s="43"/>
       <c r="C4" s="44" t="s">
         <v>190</v>
@@ -5582,10 +5597,10 @@
         <v>142</v>
       </c>
       <c r="F4" s="43"/>
-      <c r="G4" s="151"/>
-      <c r="H4" s="152"/>
-      <c r="I4" s="151"/>
-      <c r="J4" s="152"/>
+      <c r="G4" s="153"/>
+      <c r="H4" s="154"/>
+      <c r="I4" s="153"/>
+      <c r="J4" s="154"/>
       <c r="L4" s="48" t="s">
         <v>16</v>
       </c>
@@ -5611,17 +5626,21 @@
         <v>23</v>
       </c>
       <c r="T4" s="49" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="30" customHeight="1">
-      <c r="A5" s="162"/>
+      <c r="A5" s="152"/>
       <c r="B5" s="43"/>
       <c r="C5" s="50" t="s">
-        <v>245</v>
-      </c>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
+        <v>98</v>
+      </c>
+      <c r="D5" s="51" t="s">
+        <v>308</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="F5" s="43"/>
       <c r="G5" s="52"/>
       <c r="H5" s="53"/>
@@ -5646,32 +5665,32 @@
         <v>27</v>
       </c>
       <c r="R5" s="49" t="s">
+        <v>250</v>
+      </c>
+      <c r="S5" s="49" t="s">
         <v>251</v>
       </c>
-      <c r="S5" s="49" t="s">
+      <c r="T5" s="49" t="s">
         <v>252</v>
       </c>
-      <c r="T5" s="49" t="s">
-        <v>253</v>
-      </c>
     </row>
     <row r="6" spans="1:20" ht="30" customHeight="1">
-      <c r="A6" s="162"/>
+      <c r="A6" s="152"/>
       <c r="B6" s="43"/>
       <c r="C6" s="50" t="s">
         <v>97</v>
       </c>
       <c r="D6" s="51" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E6" s="49" t="s">
         <v>27</v>
       </c>
       <c r="F6" s="43"/>
-      <c r="G6" s="151"/>
-      <c r="H6" s="152"/>
-      <c r="I6" s="151"/>
-      <c r="J6" s="152"/>
+      <c r="G6" s="153"/>
+      <c r="H6" s="154"/>
+      <c r="I6" s="153"/>
+      <c r="J6" s="154"/>
       <c r="L6" s="54" t="s">
         <v>62</v>
       </c>
@@ -5682,7 +5701,7 @@
         <v>6</v>
       </c>
       <c r="O6" s="49" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="P6" s="49" t="s">
         <v>26</v>
@@ -5691,17 +5710,17 @@
         <v>27</v>
       </c>
       <c r="R6" s="49" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="S6" s="49" t="s">
         <v>61</v>
       </c>
       <c r="T6" s="49" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="30" customHeight="1">
-      <c r="A7" s="156" t="s">
+      <c r="A7" s="158" t="s">
         <v>82</v>
       </c>
       <c r="B7" s="43"/>
@@ -5709,16 +5728,16 @@
         <v>97</v>
       </c>
       <c r="D7" s="51" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E7" s="49" t="s">
         <v>27</v>
       </c>
       <c r="F7" s="51"/>
-      <c r="G7" s="151"/>
-      <c r="H7" s="152"/>
-      <c r="I7" s="151"/>
-      <c r="J7" s="152"/>
+      <c r="G7" s="153"/>
+      <c r="H7" s="154"/>
+      <c r="I7" s="153"/>
+      <c r="J7" s="154"/>
       <c r="L7" s="54" t="s">
         <v>65</v>
       </c>
@@ -5738,23 +5757,23 @@
         <v>27</v>
       </c>
       <c r="R7" s="49" t="s">
+        <v>257</v>
+      </c>
+      <c r="S7" s="49" t="s">
         <v>258</v>
       </c>
-      <c r="S7" s="49" t="s">
-        <v>259</v>
-      </c>
       <c r="T7" s="49" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="30" customHeight="1">
-      <c r="A8" s="157"/>
+      <c r="A8" s="159"/>
       <c r="B8" s="43"/>
       <c r="C8" s="50" t="s">
         <v>98</v>
       </c>
       <c r="D8" s="51" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E8" s="49" t="s">
         <v>27</v>
@@ -5774,7 +5793,7 @@
         <v>6</v>
       </c>
       <c r="O8" s="49" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="P8" s="49" t="s">
         <v>26</v>
@@ -5783,17 +5802,17 @@
         <v>27</v>
       </c>
       <c r="R8" s="49" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="S8" s="49" t="s">
         <v>64</v>
       </c>
       <c r="T8" s="49" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="30" customHeight="1">
-      <c r="A9" s="158"/>
+      <c r="A9" s="160"/>
       <c r="B9" s="43"/>
       <c r="C9" s="50" t="s">
         <v>183</v>
@@ -5828,17 +5847,17 @@
         <v>27</v>
       </c>
       <c r="R9" s="49" t="s">
+        <v>262</v>
+      </c>
+      <c r="S9" s="49" t="s">
         <v>263</v>
       </c>
-      <c r="S9" s="49" t="s">
-        <v>264</v>
-      </c>
       <c r="T9" s="49" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="30" customHeight="1">
-      <c r="A10" s="162" t="s">
+      <c r="A10" s="152" t="s">
         <v>83</v>
       </c>
       <c r="B10" s="43"/>
@@ -5852,10 +5871,10 @@
         <v>27</v>
       </c>
       <c r="F10" s="51"/>
-      <c r="G10" s="151"/>
-      <c r="H10" s="152"/>
-      <c r="I10" s="151"/>
-      <c r="J10" s="152"/>
+      <c r="G10" s="153"/>
+      <c r="H10" s="154"/>
+      <c r="I10" s="153"/>
+      <c r="J10" s="154"/>
       <c r="L10" s="54" t="s">
         <v>72</v>
       </c>
@@ -5881,28 +5900,28 @@
         <v>71</v>
       </c>
       <c r="T10" s="49" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="24.95" customHeight="1">
-      <c r="A11" s="162"/>
+      <c r="A11" s="152"/>
       <c r="B11" s="43"/>
       <c r="C11" s="44" t="s">
         <v>98</v>
       </c>
       <c r="D11" s="47" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E11" s="55" t="s">
         <v>27</v>
       </c>
       <c r="F11" s="56"/>
-      <c r="G11" s="151"/>
-      <c r="H11" s="152"/>
-      <c r="I11" s="151"/>
-      <c r="J11" s="152"/>
+      <c r="G11" s="153"/>
+      <c r="H11" s="154"/>
+      <c r="I11" s="153"/>
+      <c r="J11" s="154"/>
       <c r="L11" s="54" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="M11" s="49">
         <v>54</v>
@@ -5926,26 +5945,26 @@
         <v>75</v>
       </c>
       <c r="T11" s="49" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="24.95" customHeight="1">
-      <c r="A12" s="162"/>
+      <c r="A12" s="152"/>
       <c r="B12" s="43"/>
       <c r="C12" s="44" t="s">
         <v>183</v>
       </c>
       <c r="D12" s="47" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E12" s="55" t="s">
         <v>27</v>
       </c>
       <c r="F12" s="56"/>
-      <c r="G12" s="151"/>
-      <c r="H12" s="152"/>
-      <c r="I12" s="151"/>
-      <c r="J12" s="152"/>
+      <c r="G12" s="153"/>
+      <c r="H12" s="154"/>
+      <c r="I12" s="153"/>
+      <c r="J12" s="154"/>
       <c r="L12" s="57"/>
       <c r="O12" s="58"/>
       <c r="P12" s="58"/>
@@ -5953,12 +5972,12 @@
       <c r="T12" s="59"/>
     </row>
     <row r="13" spans="1:20" ht="24.95" customHeight="1">
-      <c r="A13" s="153" t="s">
-        <v>269</v>
+      <c r="A13" s="161" t="s">
+        <v>268</v>
       </c>
       <c r="B13" s="60"/>
       <c r="C13" s="60" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D13" s="51"/>
       <c r="E13" s="49"/>
@@ -5980,10 +5999,10 @@
       <c r="T13" s="59"/>
     </row>
     <row r="14" spans="1:20" ht="24.95" customHeight="1">
-      <c r="A14" s="154"/>
+      <c r="A14" s="162"/>
       <c r="B14" s="60"/>
       <c r="C14" s="60" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D14" s="51"/>
       <c r="E14" s="51"/>
@@ -6005,13 +6024,13 @@
       <c r="T14" s="59"/>
     </row>
     <row r="15" spans="1:20" ht="24.95" customHeight="1">
-      <c r="A15" s="154"/>
+      <c r="A15" s="162"/>
       <c r="B15" s="60"/>
       <c r="C15" s="63" t="s">
+        <v>271</v>
+      </c>
+      <c r="D15" s="47" t="s">
         <v>272</v>
-      </c>
-      <c r="D15" s="47" t="s">
-        <v>273</v>
       </c>
       <c r="E15" s="55" t="s">
         <v>27</v>
@@ -6022,7 +6041,7 @@
       <c r="I15" s="52"/>
       <c r="J15" s="53"/>
       <c r="L15" s="61" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="M15" s="61"/>
       <c r="N15" s="62" t="s">
@@ -6034,13 +6053,13 @@
       <c r="T15" s="59"/>
     </row>
     <row r="16" spans="1:20" ht="24.95" customHeight="1">
-      <c r="A16" s="154"/>
+      <c r="A16" s="162"/>
       <c r="B16" s="61" t="s">
         <v>109</v>
       </c>
       <c r="C16" s="60"/>
       <c r="D16" s="64" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E16" s="64" t="s">
         <v>25</v>
@@ -6051,7 +6070,7 @@
       <c r="I16" s="52"/>
       <c r="J16" s="53"/>
       <c r="L16" s="61" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="M16" s="62"/>
       <c r="N16" s="62" t="s">
@@ -6063,12 +6082,12 @@
       <c r="T16" s="59"/>
     </row>
     <row r="17" spans="1:19" ht="24.95" customHeight="1">
-      <c r="A17" s="155"/>
+      <c r="A17" s="163"/>
       <c r="B17" s="61" t="s">
         <v>108</v>
       </c>
       <c r="D17" s="62" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E17" s="62" t="s">
         <v>25</v>
@@ -6082,12 +6101,12 @@
       <c r="O17" s="58"/>
     </row>
     <row r="18" spans="1:19" ht="24.95" customHeight="1">
-      <c r="A18" s="153" t="s">
-        <v>278</v>
+      <c r="A18" s="161" t="s">
+        <v>277</v>
       </c>
       <c r="B18" s="60"/>
       <c r="C18" s="56" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D18" s="51"/>
       <c r="E18" s="49"/>
@@ -6100,20 +6119,20 @@
         <v>109</v>
       </c>
       <c r="M18" s="41" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="N18" s="62" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="O18" s="62" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="24.95" customHeight="1">
-      <c r="A19" s="154"/>
+      <c r="A19" s="162"/>
       <c r="B19" s="60"/>
       <c r="C19" s="60" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D19" s="51"/>
       <c r="E19" s="51"/>
@@ -6126,20 +6145,20 @@
         <v>108</v>
       </c>
       <c r="M19" s="41" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="N19" s="62" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="O19" s="62" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="24.95" customHeight="1">
-      <c r="A20" s="154"/>
+      <c r="A20" s="162"/>
       <c r="B20" s="60"/>
       <c r="C20" s="60" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D20" s="47" t="s">
         <v>66</v>
@@ -6155,13 +6174,13 @@
       <c r="M20" s="65"/>
     </row>
     <row r="21" spans="1:19" ht="24.95" customHeight="1">
-      <c r="A21" s="154"/>
+      <c r="A21" s="162"/>
       <c r="B21" s="61" t="s">
         <v>109</v>
       </c>
       <c r="C21" s="61"/>
       <c r="D21" s="64" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E21" s="64" t="s">
         <v>25</v>
@@ -6175,23 +6194,23 @@
         <v>109</v>
       </c>
       <c r="M21" s="41" t="s">
+        <v>277</v>
+      </c>
+      <c r="N21" s="62" t="s">
         <v>278</v>
-      </c>
-      <c r="N21" s="62" t="s">
-        <v>279</v>
       </c>
       <c r="O21" s="62" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="24.95" customHeight="1">
-      <c r="A22" s="155"/>
+      <c r="A22" s="163"/>
       <c r="B22" s="61" t="s">
         <v>108</v>
       </c>
       <c r="C22" s="61"/>
       <c r="D22" s="64" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E22" s="64" t="s">
         <v>25</v>
@@ -6205,17 +6224,17 @@
         <v>108</v>
       </c>
       <c r="M22" s="41" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="N22" s="62" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="O22" s="62" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="24.95" customHeight="1">
-      <c r="A23" s="156" t="s">
+      <c r="A23" s="158" t="s">
         <v>84</v>
       </c>
       <c r="B23" s="43"/>
@@ -6225,17 +6244,17 @@
       <c r="D23" s="51"/>
       <c r="E23" s="51"/>
       <c r="F23" s="56"/>
-      <c r="G23" s="151"/>
-      <c r="H23" s="152"/>
-      <c r="I23" s="151"/>
-      <c r="J23" s="152"/>
+      <c r="G23" s="153"/>
+      <c r="H23" s="154"/>
+      <c r="I23" s="153"/>
+      <c r="J23" s="154"/>
       <c r="P23" s="59"/>
       <c r="Q23" s="59"/>
       <c r="R23" s="59"/>
       <c r="S23" s="59"/>
     </row>
     <row r="24" spans="1:19" ht="24.95" customHeight="1">
-      <c r="A24" s="157"/>
+      <c r="A24" s="159"/>
       <c r="B24" s="43"/>
       <c r="C24" s="50" t="s">
         <v>99</v>
@@ -6243,13 +6262,13 @@
       <c r="D24" s="51"/>
       <c r="E24" s="51"/>
       <c r="F24" s="56"/>
-      <c r="G24" s="151"/>
-      <c r="H24" s="152"/>
-      <c r="I24" s="151"/>
-      <c r="J24" s="152"/>
+      <c r="G24" s="153"/>
+      <c r="H24" s="154"/>
+      <c r="I24" s="153"/>
+      <c r="J24" s="154"/>
     </row>
     <row r="25" spans="1:19" ht="24.95" customHeight="1">
-      <c r="A25" s="157"/>
+      <c r="A25" s="159"/>
       <c r="B25" s="43"/>
       <c r="C25" s="50" t="s">
         <v>100</v>
@@ -6257,13 +6276,13 @@
       <c r="D25" s="51"/>
       <c r="E25" s="51"/>
       <c r="F25" s="56"/>
-      <c r="G25" s="151"/>
-      <c r="H25" s="152"/>
-      <c r="I25" s="151"/>
-      <c r="J25" s="152"/>
+      <c r="G25" s="153"/>
+      <c r="H25" s="154"/>
+      <c r="I25" s="153"/>
+      <c r="J25" s="154"/>
     </row>
     <row r="26" spans="1:19" ht="24.95" customHeight="1">
-      <c r="A26" s="157"/>
+      <c r="A26" s="159"/>
       <c r="B26" s="43"/>
       <c r="C26" s="50" t="s">
         <v>101</v>
@@ -6271,13 +6290,13 @@
       <c r="D26" s="51"/>
       <c r="E26" s="51"/>
       <c r="F26" s="51"/>
-      <c r="G26" s="151"/>
-      <c r="H26" s="152"/>
-      <c r="I26" s="151"/>
-      <c r="J26" s="152"/>
+      <c r="G26" s="153"/>
+      <c r="H26" s="154"/>
+      <c r="I26" s="153"/>
+      <c r="J26" s="154"/>
     </row>
     <row r="27" spans="1:19" ht="24.95" customHeight="1">
-      <c r="A27" s="157"/>
+      <c r="A27" s="159"/>
       <c r="B27" s="43"/>
       <c r="C27" s="50" t="s">
         <v>102</v>
@@ -6285,13 +6304,13 @@
       <c r="D27" s="51"/>
       <c r="E27" s="51"/>
       <c r="F27" s="51"/>
-      <c r="G27" s="151"/>
-      <c r="H27" s="152"/>
-      <c r="I27" s="151"/>
-      <c r="J27" s="152"/>
+      <c r="G27" s="153"/>
+      <c r="H27" s="154"/>
+      <c r="I27" s="153"/>
+      <c r="J27" s="154"/>
     </row>
     <row r="28" spans="1:19" ht="24.95" customHeight="1">
-      <c r="A28" s="157"/>
+      <c r="A28" s="159"/>
       <c r="B28" s="43"/>
       <c r="C28" s="50" t="s">
         <v>103</v>
@@ -6299,13 +6318,13 @@
       <c r="D28" s="51"/>
       <c r="E28" s="51"/>
       <c r="F28" s="51"/>
-      <c r="G28" s="151"/>
-      <c r="H28" s="152"/>
-      <c r="I28" s="151"/>
-      <c r="J28" s="152"/>
+      <c r="G28" s="153"/>
+      <c r="H28" s="154"/>
+      <c r="I28" s="153"/>
+      <c r="J28" s="154"/>
     </row>
     <row r="29" spans="1:19" ht="24.95" customHeight="1">
-      <c r="A29" s="157"/>
+      <c r="A29" s="159"/>
       <c r="B29" s="43"/>
       <c r="C29" s="50" t="s">
         <v>104</v>
@@ -6319,19 +6338,19 @@
       <c r="J29" s="53"/>
     </row>
     <row r="30" spans="1:19" ht="24.95" customHeight="1">
-      <c r="A30" s="158"/>
+      <c r="A30" s="160"/>
       <c r="B30" s="60" t="s">
         <v>110</v>
       </c>
       <c r="D30" s="51"/>
       <c r="E30" s="51"/>
-      <c r="G30" s="151"/>
-      <c r="H30" s="152"/>
-      <c r="I30" s="151"/>
-      <c r="J30" s="152"/>
+      <c r="G30" s="153"/>
+      <c r="H30" s="154"/>
+      <c r="I30" s="153"/>
+      <c r="J30" s="154"/>
     </row>
     <row r="31" spans="1:19" ht="24.95" customHeight="1">
-      <c r="A31" s="153" t="s">
+      <c r="A31" s="161" t="s">
         <v>85</v>
       </c>
       <c r="B31" s="66"/>
@@ -6341,13 +6360,13 @@
       <c r="D31" s="51"/>
       <c r="E31" s="51"/>
       <c r="F31" s="51"/>
-      <c r="G31" s="151"/>
-      <c r="H31" s="152"/>
-      <c r="I31" s="151"/>
-      <c r="J31" s="152"/>
+      <c r="G31" s="153"/>
+      <c r="H31" s="154"/>
+      <c r="I31" s="153"/>
+      <c r="J31" s="154"/>
     </row>
     <row r="32" spans="1:19" ht="24.95" customHeight="1">
-      <c r="A32" s="154"/>
+      <c r="A32" s="162"/>
       <c r="B32" s="66"/>
       <c r="C32" s="50" t="s">
         <v>99</v>
@@ -6355,13 +6374,13 @@
       <c r="D32" s="51"/>
       <c r="E32" s="51"/>
       <c r="F32" s="51"/>
-      <c r="G32" s="151"/>
-      <c r="H32" s="152"/>
-      <c r="I32" s="151"/>
-      <c r="J32" s="152"/>
+      <c r="G32" s="153"/>
+      <c r="H32" s="154"/>
+      <c r="I32" s="153"/>
+      <c r="J32" s="154"/>
     </row>
     <row r="33" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A33" s="154"/>
+      <c r="A33" s="162"/>
       <c r="B33" s="66"/>
       <c r="C33" s="50" t="s">
         <v>100</v>
@@ -6369,13 +6388,13 @@
       <c r="D33" s="51"/>
       <c r="E33" s="51"/>
       <c r="F33" s="51"/>
-      <c r="G33" s="151"/>
-      <c r="H33" s="152"/>
-      <c r="I33" s="151"/>
-      <c r="J33" s="152"/>
+      <c r="G33" s="153"/>
+      <c r="H33" s="154"/>
+      <c r="I33" s="153"/>
+      <c r="J33" s="154"/>
     </row>
     <row r="34" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A34" s="154"/>
+      <c r="A34" s="162"/>
       <c r="B34" s="66"/>
       <c r="C34" s="50" t="s">
         <v>101</v>
@@ -6383,13 +6402,13 @@
       <c r="D34" s="51"/>
       <c r="E34" s="51"/>
       <c r="F34" s="51"/>
-      <c r="G34" s="151"/>
-      <c r="H34" s="152"/>
-      <c r="I34" s="151"/>
-      <c r="J34" s="152"/>
+      <c r="G34" s="153"/>
+      <c r="H34" s="154"/>
+      <c r="I34" s="153"/>
+      <c r="J34" s="154"/>
     </row>
     <row r="35" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A35" s="154"/>
+      <c r="A35" s="162"/>
       <c r="B35" s="66"/>
       <c r="C35" s="50" t="s">
         <v>102</v>
@@ -6397,13 +6416,13 @@
       <c r="D35" s="51"/>
       <c r="E35" s="51"/>
       <c r="F35" s="51"/>
-      <c r="G35" s="151"/>
-      <c r="H35" s="152"/>
-      <c r="I35" s="151"/>
-      <c r="J35" s="152"/>
+      <c r="G35" s="153"/>
+      <c r="H35" s="154"/>
+      <c r="I35" s="153"/>
+      <c r="J35" s="154"/>
     </row>
     <row r="36" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A36" s="154"/>
+      <c r="A36" s="162"/>
       <c r="B36" s="66"/>
       <c r="C36" s="50" t="s">
         <v>103</v>
@@ -6411,13 +6430,13 @@
       <c r="D36" s="51"/>
       <c r="E36" s="51"/>
       <c r="F36" s="51"/>
-      <c r="G36" s="151"/>
-      <c r="H36" s="152"/>
-      <c r="I36" s="151"/>
-      <c r="J36" s="152"/>
+      <c r="G36" s="153"/>
+      <c r="H36" s="154"/>
+      <c r="I36" s="153"/>
+      <c r="J36" s="154"/>
     </row>
     <row r="37" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A37" s="154"/>
+      <c r="A37" s="162"/>
       <c r="B37" s="66"/>
       <c r="C37" s="50" t="s">
         <v>104</v>
@@ -6425,13 +6444,13 @@
       <c r="D37" s="51"/>
       <c r="E37" s="51"/>
       <c r="F37" s="51"/>
-      <c r="G37" s="151"/>
-      <c r="H37" s="152"/>
-      <c r="I37" s="151"/>
-      <c r="J37" s="152"/>
+      <c r="G37" s="153"/>
+      <c r="H37" s="154"/>
+      <c r="I37" s="153"/>
+      <c r="J37" s="154"/>
     </row>
     <row r="38" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A38" s="154"/>
+      <c r="A38" s="162"/>
       <c r="B38" s="66"/>
       <c r="C38" s="50" t="s">
         <v>105</v>
@@ -6445,16 +6464,16 @@
       <c r="J38" s="53"/>
     </row>
     <row r="39" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A39" s="155"/>
+      <c r="A39" s="163"/>
       <c r="B39" s="60" t="s">
         <v>110</v>
       </c>
       <c r="D39" s="51"/>
       <c r="E39" s="51"/>
-      <c r="G39" s="151"/>
-      <c r="H39" s="152"/>
-      <c r="I39" s="151"/>
-      <c r="J39" s="152"/>
+      <c r="G39" s="153"/>
+      <c r="H39" s="154"/>
+      <c r="I39" s="153"/>
+      <c r="J39" s="154"/>
     </row>
     <row r="40" spans="1:10" ht="35.1" customHeight="1">
       <c r="A40" s="60" t="s">
@@ -6467,10 +6486,10 @@
       <c r="D40" s="51"/>
       <c r="E40" s="51"/>
       <c r="F40" s="51"/>
-      <c r="G40" s="151"/>
-      <c r="H40" s="152"/>
-      <c r="I40" s="151"/>
-      <c r="J40" s="152"/>
+      <c r="G40" s="153"/>
+      <c r="H40" s="154"/>
+      <c r="I40" s="153"/>
+      <c r="J40" s="154"/>
     </row>
     <row r="41" spans="1:10" ht="24.95" customHeight="1">
       <c r="A41" s="60" t="s">
@@ -6478,21 +6497,21 @@
       </c>
       <c r="B41" s="60"/>
       <c r="C41" s="50" t="s">
+        <v>280</v>
+      </c>
+      <c r="D41" s="47" t="s">
         <v>281</v>
-      </c>
-      <c r="D41" s="47" t="s">
-        <v>282</v>
       </c>
       <c r="E41" s="55" t="s">
         <v>27</v>
       </c>
       <c r="F41" s="47" t="s">
-        <v>260</v>
-      </c>
-      <c r="G41" s="151"/>
-      <c r="H41" s="152"/>
-      <c r="I41" s="151"/>
-      <c r="J41" s="152"/>
+        <v>259</v>
+      </c>
+      <c r="G41" s="153"/>
+      <c r="H41" s="154"/>
+      <c r="I41" s="153"/>
+      <c r="J41" s="154"/>
     </row>
     <row r="42" spans="1:10" ht="24.95" customHeight="1">
       <c r="A42" s="60" t="s">
@@ -6513,10 +6532,10 @@
       <c r="F42" s="64" t="s">
         <v>129</v>
       </c>
-      <c r="G42" s="151"/>
-      <c r="H42" s="152"/>
-      <c r="I42" s="151"/>
-      <c r="J42" s="152"/>
+      <c r="G42" s="153"/>
+      <c r="H42" s="154"/>
+      <c r="I42" s="153"/>
+      <c r="J42" s="154"/>
     </row>
     <row r="43" spans="1:10" ht="37.5">
       <c r="A43" s="60" t="s">
@@ -6537,10 +6556,10 @@
       <c r="F43" s="64" t="s">
         <v>129</v>
       </c>
-      <c r="G43" s="151"/>
-      <c r="H43" s="152"/>
-      <c r="I43" s="151"/>
-      <c r="J43" s="152"/>
+      <c r="G43" s="153"/>
+      <c r="H43" s="154"/>
+      <c r="I43" s="153"/>
+      <c r="J43" s="154"/>
     </row>
     <row r="44" spans="1:10" ht="37.5">
       <c r="A44" s="60" t="s">
@@ -6561,10 +6580,10 @@
       <c r="F44" s="64" t="s">
         <v>128</v>
       </c>
-      <c r="G44" s="151"/>
-      <c r="H44" s="152"/>
-      <c r="I44" s="151"/>
-      <c r="J44" s="152"/>
+      <c r="G44" s="153"/>
+      <c r="H44" s="154"/>
+      <c r="I44" s="153"/>
+      <c r="J44" s="154"/>
     </row>
     <row r="45" spans="1:10" ht="37.5">
       <c r="A45" s="60" t="s">
@@ -6585,10 +6604,10 @@
       <c r="F45" s="64" t="s">
         <v>128</v>
       </c>
-      <c r="G45" s="151"/>
-      <c r="H45" s="152"/>
-      <c r="I45" s="151"/>
-      <c r="J45" s="152"/>
+      <c r="G45" s="153"/>
+      <c r="H45" s="154"/>
+      <c r="I45" s="153"/>
+      <c r="J45" s="154"/>
     </row>
     <row r="46" spans="1:10" ht="37.5">
       <c r="A46" s="60" t="s">
@@ -6609,10 +6628,10 @@
       <c r="F46" s="64" t="s">
         <v>128</v>
       </c>
-      <c r="G46" s="151"/>
-      <c r="H46" s="152"/>
-      <c r="I46" s="151"/>
-      <c r="J46" s="152"/>
+      <c r="G46" s="153"/>
+      <c r="H46" s="154"/>
+      <c r="I46" s="153"/>
+      <c r="J46" s="154"/>
     </row>
     <row r="47" spans="1:10" ht="37.5">
       <c r="A47" s="60" t="s">
@@ -6625,7 +6644,7 @@
         <v>107</v>
       </c>
       <c r="D47" s="47" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E47" s="64" t="s">
         <v>25</v>
@@ -6633,10 +6652,10 @@
       <c r="F47" s="64" t="s">
         <v>129</v>
       </c>
-      <c r="G47" s="151"/>
-      <c r="H47" s="152"/>
-      <c r="I47" s="151"/>
-      <c r="J47" s="152"/>
+      <c r="G47" s="153"/>
+      <c r="H47" s="154"/>
+      <c r="I47" s="153"/>
+      <c r="J47" s="154"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="60" t="s">
@@ -6647,10 +6666,10 @@
       <c r="D48" s="51"/>
       <c r="E48" s="51"/>
       <c r="F48" s="62"/>
-      <c r="G48" s="151"/>
-      <c r="H48" s="152"/>
-      <c r="I48" s="151"/>
-      <c r="J48" s="152"/>
+      <c r="G48" s="153"/>
+      <c r="H48" s="154"/>
+      <c r="I48" s="153"/>
+      <c r="J48" s="154"/>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="60" t="s">
@@ -6661,10 +6680,10 @@
       <c r="D49" s="51"/>
       <c r="E49" s="51"/>
       <c r="F49" s="51"/>
-      <c r="G49" s="151"/>
-      <c r="H49" s="152"/>
-      <c r="I49" s="151"/>
-      <c r="J49" s="152"/>
+      <c r="G49" s="153"/>
+      <c r="H49" s="154"/>
+      <c r="I49" s="153"/>
+      <c r="J49" s="154"/>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="60"/>
@@ -6675,20 +6694,73 @@
       <c r="D50" s="60"/>
       <c r="E50" s="60"/>
       <c r="F50" s="60"/>
-      <c r="G50" s="151"/>
-      <c r="H50" s="152"/>
-      <c r="I50" s="151"/>
-      <c r="J50" s="152"/>
+      <c r="G50" s="153"/>
+      <c r="H50" s="154"/>
+      <c r="I50" s="153"/>
+      <c r="J50" s="154"/>
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="A23:A30"/>
+    <mergeCell ref="A31:A39"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="G11:H11"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="A3:A6"/>
@@ -6698,66 +6770,13 @@
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="A23:A30"/>
-    <mergeCell ref="A31:A39"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I10:J10"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6767,10 +6786,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A4B727F-DBFB-44AA-A62D-48CC65DAE88F}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6785,23 +6804,23 @@
     <col min="8" max="8" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="163" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="164" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="163"/>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-    </row>
-    <row r="3" spans="1:9" ht="30">
+      <c r="B1" s="164"/>
+      <c r="C1" s="164"/>
+      <c r="D1" s="164"/>
+      <c r="E1" s="164"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="164"/>
+      <c r="B2" s="164"/>
+      <c r="C2" s="164"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="164"/>
+    </row>
+    <row r="3" spans="1:10" ht="30">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -6827,10 +6846,10 @@
         <v>23</v>
       </c>
       <c r="I3" s="108" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="30">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30">
       <c r="A4" s="3" t="s">
         <v>139</v>
       </c>
@@ -6856,10 +6875,10 @@
         <v>144</v>
       </c>
       <c r="I4" s="107" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30">
       <c r="A5" s="3" t="s">
         <v>112</v>
       </c>
@@ -6885,10 +6904,10 @@
         <v>147</v>
       </c>
       <c r="I5" s="107" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="30">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="30">
       <c r="A6" s="3" t="s">
         <v>81</v>
       </c>
@@ -6914,12 +6933,12 @@
         <v>150</v>
       </c>
       <c r="I6" s="107" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="30">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="30">
       <c r="A7" s="106" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B7" s="4">
         <v>2</v>
@@ -6928,7 +6947,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>141</v>
@@ -6937,18 +6956,18 @@
         <v>142</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I7" s="107" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="30">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="30">
       <c r="A8" s="106" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B8" s="4">
         <v>2</v>
@@ -6957,7 +6976,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>141</v>
@@ -6966,18 +6985,80 @@
         <v>142</v>
       </c>
       <c r="G8" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="I8" s="107" t="s">
         <v>305</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="I8" s="107" t="s">
-        <v>306</v>
-      </c>
+    </row>
+    <row r="11" spans="1:10" ht="37.5">
+      <c r="A11" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="157" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="157"/>
+      <c r="I11" s="157" t="s">
+        <v>111</v>
+      </c>
+      <c r="J11" s="157"/>
+    </row>
+    <row r="12" spans="1:10" ht="18.75">
+      <c r="A12" s="42"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="165"/>
+      <c r="E12" s="165"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="166"/>
+      <c r="H12" s="167"/>
+      <c r="I12" s="166"/>
+      <c r="J12" s="167"/>
+    </row>
+    <row r="13" spans="1:10" ht="30">
+      <c r="A13" s="106" t="s">
+        <v>297</v>
+      </c>
+      <c r="B13" s="43"/>
+      <c r="C13" s="50" t="s">
+        <v>309</v>
+      </c>
+      <c r="D13" s="51" t="s">
+        <v>310</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F13" s="43"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="53"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:E2"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
vpn linux server és győr között, a soproni vezeték nélküli routernél módosítva az ip cím
</commit_message>
<xml_diff>
--- a/IP_cim_kiosztas_akutális.xlsx
+++ b/IP_cim_kiosztas_akutális.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Üzemeltető\Vizsgaremek\Uzemelteto_vizsgaremek_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F12DFB0-F835-4D13-B258-B1AE9F833DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993A0B47-C376-42D7-8C8E-D83D356AEFF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{5DEB228F-9A24-4144-85FF-8E6948A8BA71}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{5DEB228F-9A24-4144-85FF-8E6948A8BA71}"/>
   </bookViews>
   <sheets>
     <sheet name="Központi Iroda" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="ipv6 pool" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="345">
   <si>
     <t>Központi Iroda</t>
   </si>
@@ -978,9 +977,6 @@
     <t>255.255.255.253</t>
   </si>
   <si>
-    <t>192.168.1.1 - 192.168.1.62</t>
-  </si>
-  <si>
     <t>192.168.1.2</t>
   </si>
   <si>
@@ -1066,6 +1062,15 @@
   </si>
   <si>
     <t>192.168.5.126</t>
+  </si>
+  <si>
+    <t>192.168.2.0</t>
+  </si>
+  <si>
+    <t>192.168.2.1 - 192.168.2.62</t>
+  </si>
+  <si>
+    <t>192.168.2.63</t>
   </si>
 </sst>
 </file>
@@ -2206,6 +2211,33 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2245,128 +2277,101 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2726,20 +2731,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="40.5" customHeight="1" thickBot="1">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="128" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="130" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="123" t="s">
+      <c r="B2" s="132" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -2748,7 +2753,7 @@
       <c r="D2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="128" t="s">
+      <c r="E2" s="137" t="s">
         <v>55</v>
       </c>
       <c r="F2" s="14" t="s">
@@ -2756,13 +2761,13 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="122"/>
-      <c r="B3" s="124"/>
-      <c r="C3" s="125" t="s">
+      <c r="A3" s="131"/>
+      <c r="B3" s="133"/>
+      <c r="C3" s="134" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="126"/>
-      <c r="E3" s="129"/>
+      <c r="D3" s="135"/>
+      <c r="E3" s="138"/>
       <c r="F3" s="15" t="s">
         <v>6</v>
       </c>
@@ -2782,7 +2787,7 @@
       <c r="F4" s="28"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1">
-      <c r="A5" s="118" t="s">
+      <c r="A5" s="127" t="s">
         <v>138</v>
       </c>
       <c r="B5" s="24" t="s">
@@ -2798,7 +2803,7 @@
       <c r="F5" s="25"/>
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1">
-      <c r="A6" s="118"/>
+      <c r="A6" s="127"/>
       <c r="B6" s="1" t="s">
         <v>152</v>
       </c>
@@ -2821,7 +2826,7 @@
       <c r="Q6" s="17"/>
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1">
-      <c r="A7" s="118"/>
+      <c r="A7" s="127"/>
       <c r="B7" s="1" t="s">
         <v>153</v>
       </c>
@@ -2844,7 +2849,7 @@
       <c r="Q7" s="17"/>
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1">
-      <c r="A8" s="117" t="s">
+      <c r="A8" s="126" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="26"/>
@@ -2863,7 +2868,7 @@
       <c r="Q8" s="17"/>
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1">
-      <c r="A9" s="127"/>
+      <c r="A9" s="136"/>
       <c r="B9" s="26"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -2880,7 +2885,7 @@
       <c r="Q9" s="17"/>
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1">
-      <c r="A10" s="117" t="s">
+      <c r="A10" s="126" t="s">
         <v>154</v>
       </c>
       <c r="B10" s="27" t="s">
@@ -2905,7 +2910,7 @@
       <c r="Q10" s="17"/>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" thickBot="1">
-      <c r="A11" s="118"/>
+      <c r="A11" s="127"/>
       <c r="B11" s="27" t="s">
         <v>157</v>
       </c>
@@ -2919,7 +2924,7 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1">
-      <c r="A12" s="118"/>
+      <c r="A12" s="127"/>
       <c r="B12" s="27" t="s">
         <v>159</v>
       </c>
@@ -2931,39 +2936,39 @@
       </c>
       <c r="E12" s="28"/>
       <c r="F12" s="8"/>
-      <c r="I12" s="133" t="s">
+      <c r="I12" s="124" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="135" t="s">
+      <c r="J12" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="135" t="s">
+      <c r="K12" s="120" t="s">
         <v>18</v>
       </c>
-      <c r="L12" s="135" t="s">
+      <c r="L12" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="M12" s="135" t="s">
+      <c r="M12" s="120" t="s">
         <v>20</v>
       </c>
-      <c r="N12" s="135" t="s">
+      <c r="N12" s="120" t="s">
         <v>21</v>
       </c>
-      <c r="O12" s="135" t="s">
+      <c r="O12" s="120" t="s">
         <v>22</v>
       </c>
-      <c r="P12" s="135" t="s">
+      <c r="P12" s="120" t="s">
         <v>23</v>
       </c>
-      <c r="Q12" s="135" t="s">
+      <c r="Q12" s="120" t="s">
         <v>55</v>
       </c>
-      <c r="R12" s="137" t="s">
+      <c r="R12" s="122" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1">
-      <c r="A13" s="118"/>
+      <c r="A13" s="127"/>
       <c r="B13" s="27" t="s">
         <v>161</v>
       </c>
@@ -2975,19 +2980,19 @@
       </c>
       <c r="E13" s="28"/>
       <c r="F13" s="8"/>
-      <c r="I13" s="134"/>
-      <c r="J13" s="136"/>
-      <c r="K13" s="136"/>
-      <c r="L13" s="136"/>
-      <c r="M13" s="136"/>
-      <c r="N13" s="136"/>
-      <c r="O13" s="136"/>
-      <c r="P13" s="136"/>
-      <c r="Q13" s="136"/>
-      <c r="R13" s="138"/>
+      <c r="I13" s="125"/>
+      <c r="J13" s="121"/>
+      <c r="K13" s="121"/>
+      <c r="L13" s="121"/>
+      <c r="M13" s="121"/>
+      <c r="N13" s="121"/>
+      <c r="O13" s="121"/>
+      <c r="P13" s="121"/>
+      <c r="Q13" s="121"/>
+      <c r="R13" s="123"/>
     </row>
     <row r="14" spans="1:18" ht="15" customHeight="1">
-      <c r="A14" s="118"/>
+      <c r="A14" s="127"/>
       <c r="B14" s="27" t="s">
         <v>163</v>
       </c>
@@ -2999,113 +3004,113 @@
       </c>
       <c r="E14" s="28"/>
       <c r="F14" s="8"/>
-      <c r="I14" s="131" t="s">
+      <c r="I14" s="117" t="s">
         <v>33</v>
       </c>
-      <c r="J14" s="131">
+      <c r="J14" s="117">
         <v>7</v>
       </c>
-      <c r="K14" s="131">
+      <c r="K14" s="117">
         <v>30</v>
       </c>
-      <c r="L14" s="130" t="s">
+      <c r="L14" s="118" t="s">
         <v>39</v>
       </c>
-      <c r="M14" s="131" t="s">
+      <c r="M14" s="117" t="s">
         <v>31</v>
       </c>
-      <c r="N14" s="132" t="s">
+      <c r="N14" s="119" t="s">
         <v>38</v>
       </c>
-      <c r="O14" s="130" t="s">
+      <c r="O14" s="118" t="s">
         <v>40</v>
       </c>
-      <c r="P14" s="130" t="s">
+      <c r="P14" s="118" t="s">
         <v>41</v>
       </c>
-      <c r="Q14" s="130" t="s">
+      <c r="Q14" s="118" t="s">
         <v>51</v>
       </c>
-      <c r="R14" s="130" t="s">
+      <c r="R14" s="118" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="15" customHeight="1">
-      <c r="A15" s="118"/>
+      <c r="A15" s="127"/>
       <c r="B15" s="27"/>
       <c r="C15" s="28"/>
       <c r="D15" s="28"/>
       <c r="E15" s="28"/>
       <c r="F15" s="8"/>
-      <c r="I15" s="131"/>
-      <c r="J15" s="131"/>
-      <c r="K15" s="131"/>
-      <c r="L15" s="130"/>
-      <c r="M15" s="131"/>
-      <c r="N15" s="132"/>
-      <c r="O15" s="130"/>
-      <c r="P15" s="130"/>
-      <c r="Q15" s="130"/>
-      <c r="R15" s="130"/>
+      <c r="I15" s="117"/>
+      <c r="J15" s="117"/>
+      <c r="K15" s="117"/>
+      <c r="L15" s="118"/>
+      <c r="M15" s="117"/>
+      <c r="N15" s="119"/>
+      <c r="O15" s="118"/>
+      <c r="P15" s="118"/>
+      <c r="Q15" s="118"/>
+      <c r="R15" s="118"/>
     </row>
     <row r="16" spans="1:18" ht="15" customHeight="1">
-      <c r="A16" s="118"/>
+      <c r="A16" s="127"/>
       <c r="B16" s="27"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="8"/>
-      <c r="I16" s="131" t="s">
+      <c r="I16" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="J16" s="131">
+      <c r="J16" s="117">
         <v>5</v>
       </c>
-      <c r="K16" s="131">
+      <c r="K16" s="117">
         <v>30</v>
       </c>
-      <c r="L16" s="130" t="s">
+      <c r="L16" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="M16" s="131" t="s">
+      <c r="M16" s="117" t="s">
         <v>31</v>
       </c>
-      <c r="N16" s="132" t="s">
+      <c r="N16" s="119" t="s">
         <v>38</v>
       </c>
-      <c r="O16" s="130" t="s">
+      <c r="O16" s="118" t="s">
         <v>43</v>
       </c>
-      <c r="P16" s="130" t="s">
+      <c r="P16" s="118" t="s">
         <v>44</v>
       </c>
-      <c r="Q16" s="130" t="s">
+      <c r="Q16" s="118" t="s">
         <v>52</v>
       </c>
-      <c r="R16" s="130" t="s">
+      <c r="R16" s="118" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="15" customHeight="1">
-      <c r="A17" s="118"/>
+      <c r="A17" s="127"/>
       <c r="B17" s="27"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="8"/>
-      <c r="I17" s="131"/>
-      <c r="J17" s="131"/>
-      <c r="K17" s="131"/>
-      <c r="L17" s="130"/>
-      <c r="M17" s="131"/>
-      <c r="N17" s="132"/>
-      <c r="O17" s="130"/>
-      <c r="P17" s="130"/>
-      <c r="Q17" s="130"/>
-      <c r="R17" s="130"/>
+      <c r="I17" s="117"/>
+      <c r="J17" s="117"/>
+      <c r="K17" s="117"/>
+      <c r="L17" s="118"/>
+      <c r="M17" s="117"/>
+      <c r="N17" s="119"/>
+      <c r="O17" s="118"/>
+      <c r="P17" s="118"/>
+      <c r="Q17" s="118"/>
+      <c r="R17" s="118"/>
     </row>
     <row r="18" spans="1:18" ht="15" customHeight="1">
-      <c r="A18" s="117" t="s">
+      <c r="A18" s="126" t="s">
         <v>165</v>
       </c>
       <c r="B18" s="27" t="s">
@@ -3119,39 +3124,39 @@
       </c>
       <c r="E18" s="28"/>
       <c r="F18" s="8"/>
-      <c r="I18" s="131" t="s">
+      <c r="I18" s="117" t="s">
         <v>35</v>
       </c>
-      <c r="J18" s="131">
+      <c r="J18" s="117">
         <v>1</v>
       </c>
-      <c r="K18" s="131">
+      <c r="K18" s="117">
         <v>6</v>
       </c>
-      <c r="L18" s="130" t="s">
+      <c r="L18" s="118" t="s">
         <v>45</v>
       </c>
-      <c r="M18" s="131" t="s">
+      <c r="M18" s="117" t="s">
         <v>26</v>
       </c>
-      <c r="N18" s="132" t="s">
+      <c r="N18" s="119" t="s">
         <v>37</v>
       </c>
-      <c r="O18" s="130" t="s">
+      <c r="O18" s="118" t="s">
         <v>46</v>
       </c>
-      <c r="P18" s="130" t="s">
+      <c r="P18" s="118" t="s">
         <v>47</v>
       </c>
-      <c r="Q18" s="130" t="s">
+      <c r="Q18" s="118" t="s">
         <v>53</v>
       </c>
-      <c r="R18" s="130" t="s">
+      <c r="R18" s="118" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="15" customHeight="1">
-      <c r="A19" s="118"/>
+      <c r="A19" s="127"/>
       <c r="B19" s="27" t="s">
         <v>157</v>
       </c>
@@ -3163,19 +3168,19 @@
       </c>
       <c r="E19" s="28"/>
       <c r="F19" s="8"/>
-      <c r="I19" s="131"/>
-      <c r="J19" s="131"/>
-      <c r="K19" s="131"/>
-      <c r="L19" s="130"/>
-      <c r="M19" s="131"/>
-      <c r="N19" s="132"/>
-      <c r="O19" s="130"/>
-      <c r="P19" s="130"/>
-      <c r="Q19" s="130"/>
-      <c r="R19" s="130"/>
+      <c r="I19" s="117"/>
+      <c r="J19" s="117"/>
+      <c r="K19" s="117"/>
+      <c r="L19" s="118"/>
+      <c r="M19" s="117"/>
+      <c r="N19" s="119"/>
+      <c r="O19" s="118"/>
+      <c r="P19" s="118"/>
+      <c r="Q19" s="118"/>
+      <c r="R19" s="118"/>
     </row>
     <row r="20" spans="1:18" ht="15" customHeight="1">
-      <c r="A20" s="118"/>
+      <c r="A20" s="127"/>
       <c r="B20" s="27" t="s">
         <v>159</v>
       </c>
@@ -3187,39 +3192,39 @@
       </c>
       <c r="E20" s="28"/>
       <c r="F20" s="8"/>
-      <c r="I20" s="131" t="s">
+      <c r="I20" s="117" t="s">
         <v>36</v>
       </c>
-      <c r="J20" s="131">
+      <c r="J20" s="117">
         <v>1</v>
       </c>
-      <c r="K20" s="131">
+      <c r="K20" s="117">
         <v>6</v>
       </c>
-      <c r="L20" s="130" t="s">
+      <c r="L20" s="118" t="s">
         <v>48</v>
       </c>
-      <c r="M20" s="131" t="s">
+      <c r="M20" s="117" t="s">
         <v>26</v>
       </c>
-      <c r="N20" s="132" t="s">
+      <c r="N20" s="119" t="s">
         <v>37</v>
       </c>
-      <c r="O20" s="130" t="s">
+      <c r="O20" s="118" t="s">
         <v>49</v>
       </c>
-      <c r="P20" s="130" t="s">
+      <c r="P20" s="118" t="s">
         <v>50</v>
       </c>
-      <c r="Q20" s="130" t="s">
+      <c r="Q20" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="R20" s="130" t="s">
+      <c r="R20" s="118" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="15" customHeight="1">
-      <c r="A21" s="118"/>
+      <c r="A21" s="127"/>
       <c r="B21" s="27" t="s">
         <v>161</v>
       </c>
@@ -3231,19 +3236,19 @@
       </c>
       <c r="E21" s="28"/>
       <c r="F21" s="8"/>
-      <c r="I21" s="131"/>
-      <c r="J21" s="131"/>
-      <c r="K21" s="131"/>
-      <c r="L21" s="130"/>
-      <c r="M21" s="131"/>
-      <c r="N21" s="132"/>
-      <c r="O21" s="130"/>
-      <c r="P21" s="130"/>
-      <c r="Q21" s="130"/>
-      <c r="R21" s="130"/>
+      <c r="I21" s="117"/>
+      <c r="J21" s="117"/>
+      <c r="K21" s="117"/>
+      <c r="L21" s="118"/>
+      <c r="M21" s="117"/>
+      <c r="N21" s="119"/>
+      <c r="O21" s="118"/>
+      <c r="P21" s="118"/>
+      <c r="Q21" s="118"/>
+      <c r="R21" s="118"/>
     </row>
     <row r="22" spans="1:18" ht="15" customHeight="1">
-      <c r="A22" s="118"/>
+      <c r="A22" s="127"/>
       <c r="B22" s="27" t="s">
         <v>163</v>
       </c>
@@ -3255,57 +3260,57 @@
       </c>
       <c r="E22" s="28"/>
       <c r="F22" s="8"/>
-      <c r="I22" s="131" t="s">
+      <c r="I22" s="117" t="s">
         <v>176</v>
       </c>
-      <c r="J22" s="131">
+      <c r="J22" s="117">
         <v>3</v>
       </c>
-      <c r="K22" s="131">
+      <c r="K22" s="117">
         <v>6</v>
       </c>
-      <c r="L22" s="130" t="s">
+      <c r="L22" s="118" t="s">
         <v>177</v>
       </c>
-      <c r="M22" s="131" t="s">
+      <c r="M22" s="117" t="s">
         <v>26</v>
       </c>
-      <c r="N22" s="132" t="s">
+      <c r="N22" s="119" t="s">
         <v>37</v>
       </c>
-      <c r="O22" s="130" t="s">
+      <c r="O22" s="118" t="s">
         <v>178</v>
       </c>
-      <c r="P22" s="130" t="s">
+      <c r="P22" s="118" t="s">
         <v>179</v>
       </c>
-      <c r="Q22" s="130" t="s">
+      <c r="Q22" s="118" t="s">
         <v>180</v>
       </c>
-      <c r="R22" s="130" t="s">
+      <c r="R22" s="118" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="15" customHeight="1">
-      <c r="A23" s="118"/>
+      <c r="A23" s="127"/>
       <c r="B23" s="27"/>
       <c r="C23" s="28"/>
       <c r="D23" s="28"/>
       <c r="E23" s="28"/>
       <c r="F23" s="8"/>
-      <c r="I23" s="131"/>
-      <c r="J23" s="131"/>
-      <c r="K23" s="131"/>
-      <c r="L23" s="130"/>
-      <c r="M23" s="131"/>
-      <c r="N23" s="132"/>
-      <c r="O23" s="130"/>
-      <c r="P23" s="130"/>
-      <c r="Q23" s="130"/>
-      <c r="R23" s="130"/>
+      <c r="I23" s="117"/>
+      <c r="J23" s="117"/>
+      <c r="K23" s="117"/>
+      <c r="L23" s="118"/>
+      <c r="M23" s="117"/>
+      <c r="N23" s="119"/>
+      <c r="O23" s="118"/>
+      <c r="P23" s="118"/>
+      <c r="Q23" s="118"/>
+      <c r="R23" s="118"/>
     </row>
     <row r="24" spans="1:18" ht="15" customHeight="1">
-      <c r="A24" s="118"/>
+      <c r="A24" s="127"/>
       <c r="B24" s="27"/>
       <c r="C24" s="28"/>
       <c r="D24" s="28"/>
@@ -3313,7 +3318,7 @@
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:18" ht="15" customHeight="1">
-      <c r="A25" s="118"/>
+      <c r="A25" s="127"/>
       <c r="B25" s="27"/>
       <c r="C25" s="28"/>
       <c r="D25" s="28"/>
@@ -3538,16 +3543,49 @@
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="R16:R17"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="O14:O15"/>
+    <mergeCell ref="P14:P15"/>
+    <mergeCell ref="Q14:Q15"/>
+    <mergeCell ref="R14:R15"/>
+    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="Q16:Q17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="O12:O13"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="Q12:Q13"/>
+    <mergeCell ref="R12:R13"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="O20:O21"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="K20:K21"/>
     <mergeCell ref="M22:M23"/>
     <mergeCell ref="R18:R19"/>
     <mergeCell ref="Q20:Q21"/>
@@ -3564,49 +3602,16 @@
     <mergeCell ref="M18:M19"/>
     <mergeCell ref="M20:M21"/>
     <mergeCell ref="N18:N19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="O20:O21"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="O12:O13"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="Q12:Q13"/>
-    <mergeCell ref="R12:R13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="R16:R17"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="O14:O15"/>
-    <mergeCell ref="P14:P15"/>
-    <mergeCell ref="Q14:Q15"/>
-    <mergeCell ref="R14:R15"/>
-    <mergeCell ref="P16:P17"/>
-    <mergeCell ref="Q16:Q17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="A10:A17"/>
-    <mergeCell ref="A18:A25"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="K18:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3617,7 +3622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B769BC50-9623-4726-8971-E5FD68E08F76}">
   <dimension ref="A1:T81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -3643,16 +3648,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="17.25">
-      <c r="A1" s="143"/>
-      <c r="B1" s="144"/>
-      <c r="C1" s="144"/>
-      <c r="D1" s="144"/>
-      <c r="E1" s="144"/>
-      <c r="F1" s="144"/>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
-      <c r="I1" s="144"/>
-      <c r="J1" s="144"/>
+      <c r="A1" s="157"/>
+      <c r="B1" s="158"/>
+      <c r="C1" s="158"/>
+      <c r="D1" s="158"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="158"/>
+      <c r="G1" s="158"/>
+      <c r="H1" s="158"/>
+      <c r="I1" s="158"/>
+      <c r="J1" s="158"/>
     </row>
     <row r="2" spans="1:20" ht="33" customHeight="1">
       <c r="A2" s="66" t="s">
@@ -3673,14 +3678,14 @@
       <c r="F2" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="145" t="s">
+      <c r="G2" s="142" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="145"/>
-      <c r="I2" s="145" t="s">
+      <c r="H2" s="142"/>
+      <c r="I2" s="142" t="s">
         <v>110</v>
       </c>
-      <c r="J2" s="145"/>
+      <c r="J2" s="142"/>
       <c r="L2" s="2" t="s">
         <v>16</v>
       </c>
@@ -3707,7 +3712,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="30">
-      <c r="A3" s="146" t="s">
+      <c r="A3" s="156" t="s">
         <v>111</v>
       </c>
       <c r="B3" s="9"/>
@@ -3721,10 +3726,10 @@
         <v>141</v>
       </c>
       <c r="F3" s="9"/>
-      <c r="G3" s="147"/>
-      <c r="H3" s="147"/>
-      <c r="I3" s="147"/>
-      <c r="J3" s="147"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
       <c r="L3" s="3" t="s">
         <v>215</v>
       </c>
@@ -3754,7 +3759,7 @@
       </c>
     </row>
     <row r="4" spans="1:20" ht="18.75" customHeight="1">
-      <c r="A4" s="146"/>
+      <c r="A4" s="156"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
         <v>96</v>
@@ -3766,10 +3771,10 @@
         <v>141</v>
       </c>
       <c r="F4" s="9"/>
-      <c r="G4" s="147"/>
-      <c r="H4" s="147"/>
-      <c r="I4" s="147"/>
-      <c r="J4" s="147"/>
+      <c r="G4" s="153"/>
+      <c r="H4" s="153"/>
+      <c r="I4" s="153"/>
+      <c r="J4" s="153"/>
       <c r="L4" s="3" t="s">
         <v>216</v>
       </c>
@@ -3799,7 +3804,7 @@
       </c>
     </row>
     <row r="5" spans="1:20" ht="27" customHeight="1">
-      <c r="A5" s="146"/>
+      <c r="A5" s="156"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9" t="s">
         <v>97</v>
@@ -3811,10 +3816,10 @@
         <v>141</v>
       </c>
       <c r="F5" s="9"/>
-      <c r="G5" s="147"/>
-      <c r="H5" s="147"/>
-      <c r="I5" s="147"/>
-      <c r="J5" s="147"/>
+      <c r="G5" s="153"/>
+      <c r="H5" s="153"/>
+      <c r="I5" s="153"/>
+      <c r="J5" s="153"/>
       <c r="L5" s="3" t="s">
         <v>285</v>
       </c>
@@ -3858,10 +3863,10 @@
         <v>141</v>
       </c>
       <c r="F6" s="35"/>
-      <c r="G6" s="142"/>
-      <c r="H6" s="142"/>
-      <c r="I6" s="142"/>
-      <c r="J6" s="142"/>
+      <c r="G6" s="151"/>
+      <c r="H6" s="151"/>
+      <c r="I6" s="151"/>
+      <c r="J6" s="151"/>
       <c r="L6" s="3" t="s">
         <v>282</v>
       </c>
@@ -3894,10 +3899,10 @@
       <c r="A7" s="70"/>
       <c r="B7" s="35"/>
       <c r="C7" s="35" t="s">
+        <v>323</v>
+      </c>
+      <c r="D7" s="35" t="s">
         <v>324</v>
-      </c>
-      <c r="D7" s="35" t="s">
-        <v>325</v>
       </c>
       <c r="E7" s="35" t="s">
         <v>25</v>
@@ -3939,10 +3944,10 @@
       <c r="A8" s="70"/>
       <c r="B8" s="35"/>
       <c r="C8" s="35" t="s">
+        <v>325</v>
+      </c>
+      <c r="D8" s="35" t="s">
         <v>326</v>
-      </c>
-      <c r="D8" s="35" t="s">
-        <v>327</v>
       </c>
       <c r="E8" s="35" t="s">
         <v>25</v>
@@ -3984,10 +3989,10 @@
       <c r="A9" s="70"/>
       <c r="B9" s="35"/>
       <c r="C9" s="35" t="s">
+        <v>327</v>
+      </c>
+      <c r="D9" s="35" t="s">
         <v>328</v>
-      </c>
-      <c r="D9" s="35" t="s">
-        <v>329</v>
       </c>
       <c r="E9" s="35" t="s">
         <v>25</v>
@@ -4047,22 +4052,22 @@
         <v>141</v>
       </c>
       <c r="F11" s="71"/>
-      <c r="G11" s="153"/>
-      <c r="H11" s="153"/>
-      <c r="I11" s="153"/>
-      <c r="J11" s="153"/>
+      <c r="G11" s="139"/>
+      <c r="H11" s="139"/>
+      <c r="I11" s="139"/>
+      <c r="J11" s="139"/>
       <c r="S11" s="4"/>
     </row>
     <row r="12" spans="1:20" ht="17.25">
       <c r="A12" s="79" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B12" s="79" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C12" s="79"/>
       <c r="D12" s="79" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E12" s="79" t="s">
         <v>25</v>
@@ -4088,14 +4093,14 @@
         <v>121</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>295</v>
@@ -4121,7 +4126,7 @@
         <v>119</v>
       </c>
       <c r="C14" s="74" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D14" s="73" t="s">
         <v>134</v>
@@ -4190,7 +4195,7 @@
       </c>
       <c r="C17" s="74"/>
       <c r="D17" s="73" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E17" s="73" t="s">
         <v>25</v>
@@ -4256,7 +4261,7 @@
       </c>
       <c r="C20" s="77"/>
       <c r="D20" s="16" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E20" s="16" t="s">
         <v>25</v>
@@ -4264,10 +4269,10 @@
       <c r="F20" s="77" t="s">
         <v>122</v>
       </c>
-      <c r="G20" s="140"/>
-      <c r="H20" s="140"/>
-      <c r="I20" s="140"/>
-      <c r="J20" s="140"/>
+      <c r="G20" s="149"/>
+      <c r="H20" s="149"/>
+      <c r="I20" s="149"/>
+      <c r="J20" s="149"/>
     </row>
     <row r="21" spans="1:19" ht="16.5" customHeight="1" thickBot="1">
       <c r="A21" s="79" t="s">
@@ -4278,7 +4283,7 @@
       </c>
       <c r="C21" s="81"/>
       <c r="D21" s="16" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E21" s="80" t="s">
         <v>25</v>
@@ -4286,10 +4291,10 @@
       <c r="F21" s="81" t="s">
         <v>122</v>
       </c>
-      <c r="G21" s="141"/>
-      <c r="H21" s="141"/>
-      <c r="I21" s="141"/>
-      <c r="J21" s="141"/>
+      <c r="G21" s="146"/>
+      <c r="H21" s="146"/>
+      <c r="I21" s="146"/>
+      <c r="J21" s="146"/>
       <c r="S21" s="6"/>
     </row>
     <row r="22" spans="1:19" ht="35.25" thickBot="1">
@@ -4299,12 +4304,12 @@
       <c r="D22" s="84"/>
       <c r="E22" s="84"/>
       <c r="F22" s="84"/>
-      <c r="G22" s="149"/>
-      <c r="H22" s="149"/>
-      <c r="I22" s="149"/>
-      <c r="J22" s="150"/>
+      <c r="G22" s="147"/>
+      <c r="H22" s="147"/>
+      <c r="I22" s="147"/>
+      <c r="J22" s="148"/>
       <c r="L22" s="111" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="M22" s="60"/>
       <c r="N22" s="4" t="s">
@@ -4321,12 +4326,12 @@
       <c r="D23" s="34"/>
       <c r="E23" s="34"/>
       <c r="F23" s="34"/>
-      <c r="G23" s="139"/>
-      <c r="H23" s="139"/>
-      <c r="I23" s="139"/>
-      <c r="J23" s="139"/>
+      <c r="G23" s="140"/>
+      <c r="H23" s="140"/>
+      <c r="I23" s="140"/>
+      <c r="J23" s="140"/>
       <c r="L23" s="112" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="M23" s="60"/>
       <c r="N23" s="4" t="s">
@@ -4343,12 +4348,12 @@
       <c r="D24" s="34"/>
       <c r="E24" s="34"/>
       <c r="F24" s="34"/>
-      <c r="G24" s="139"/>
-      <c r="H24" s="139"/>
-      <c r="I24" s="139"/>
-      <c r="J24" s="139"/>
+      <c r="G24" s="140"/>
+      <c r="H24" s="140"/>
+      <c r="I24" s="140"/>
+      <c r="J24" s="140"/>
       <c r="L24" s="113" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="N24" s="4" t="s">
         <v>57</v>
@@ -4364,12 +4369,12 @@
       <c r="D25" s="34"/>
       <c r="E25" s="34"/>
       <c r="F25" s="34"/>
-      <c r="G25" s="139"/>
-      <c r="H25" s="139"/>
-      <c r="I25" s="139"/>
-      <c r="J25" s="139"/>
+      <c r="G25" s="140"/>
+      <c r="H25" s="140"/>
+      <c r="I25" s="140"/>
+      <c r="J25" s="140"/>
       <c r="L25" s="111" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="M25" s="114"/>
       <c r="N25" s="115" t="s">
@@ -4386,12 +4391,12 @@
       <c r="D26" s="34"/>
       <c r="E26" s="34"/>
       <c r="F26" s="34"/>
-      <c r="G26" s="139"/>
-      <c r="H26" s="139"/>
-      <c r="I26" s="139"/>
-      <c r="J26" s="139"/>
+      <c r="G26" s="140"/>
+      <c r="H26" s="140"/>
+      <c r="I26" s="140"/>
+      <c r="J26" s="140"/>
       <c r="L26" s="112" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="M26" s="61"/>
       <c r="N26" s="116" t="s">
@@ -4408,12 +4413,12 @@
       <c r="D27" s="34"/>
       <c r="E27" s="34"/>
       <c r="F27" s="34"/>
-      <c r="G27" s="139"/>
-      <c r="H27" s="139"/>
-      <c r="I27" s="139"/>
-      <c r="J27" s="139"/>
+      <c r="G27" s="140"/>
+      <c r="H27" s="140"/>
+      <c r="I27" s="140"/>
+      <c r="J27" s="140"/>
       <c r="L27" s="113" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="M27" s="1"/>
       <c r="N27" s="116" t="s">
@@ -4430,10 +4435,10 @@
       <c r="D28" s="34"/>
       <c r="E28" s="34"/>
       <c r="F28" s="34"/>
-      <c r="G28" s="139"/>
-      <c r="H28" s="139"/>
-      <c r="I28" s="139"/>
-      <c r="J28" s="139"/>
+      <c r="G28" s="140"/>
+      <c r="H28" s="140"/>
+      <c r="I28" s="140"/>
+      <c r="J28" s="140"/>
     </row>
     <row r="29" spans="1:19" ht="18" thickBot="1">
       <c r="A29" s="94"/>
@@ -4442,10 +4447,10 @@
       <c r="D29" s="34"/>
       <c r="E29" s="34"/>
       <c r="F29" s="34"/>
-      <c r="G29" s="139"/>
-      <c r="H29" s="139"/>
-      <c r="I29" s="139"/>
-      <c r="J29" s="139"/>
+      <c r="G29" s="140"/>
+      <c r="H29" s="140"/>
+      <c r="I29" s="140"/>
+      <c r="J29" s="140"/>
     </row>
     <row r="30" spans="1:19" ht="17.25">
       <c r="A30" s="95"/>
@@ -4454,10 +4459,10 @@
       <c r="D30" s="34"/>
       <c r="E30" s="34"/>
       <c r="F30" s="34"/>
-      <c r="G30" s="139"/>
-      <c r="H30" s="139"/>
-      <c r="I30" s="139"/>
-      <c r="J30" s="139"/>
+      <c r="G30" s="140"/>
+      <c r="H30" s="140"/>
+      <c r="I30" s="140"/>
+      <c r="J30" s="140"/>
     </row>
     <row r="31" spans="1:19" ht="17.25">
       <c r="A31" s="34"/>
@@ -4466,10 +4471,10 @@
       <c r="D31" s="34"/>
       <c r="E31" s="34"/>
       <c r="F31" s="34"/>
-      <c r="G31" s="139"/>
-      <c r="H31" s="139"/>
-      <c r="I31" s="139"/>
-      <c r="J31" s="139"/>
+      <c r="G31" s="140"/>
+      <c r="H31" s="140"/>
+      <c r="I31" s="140"/>
+      <c r="J31" s="140"/>
     </row>
     <row r="32" spans="1:19" ht="17.25">
       <c r="A32" s="34"/>
@@ -4478,10 +4483,10 @@
       <c r="D32" s="34"/>
       <c r="E32" s="34"/>
       <c r="F32" s="34"/>
-      <c r="G32" s="139"/>
-      <c r="H32" s="139"/>
-      <c r="I32" s="139"/>
-      <c r="J32" s="139"/>
+      <c r="G32" s="140"/>
+      <c r="H32" s="140"/>
+      <c r="I32" s="140"/>
+      <c r="J32" s="140"/>
     </row>
     <row r="33" spans="1:10" ht="17.25">
       <c r="A33" s="34"/>
@@ -4490,10 +4495,10 @@
       <c r="D33" s="34"/>
       <c r="E33" s="34"/>
       <c r="F33" s="34"/>
-      <c r="G33" s="139"/>
-      <c r="H33" s="139"/>
-      <c r="I33" s="139"/>
-      <c r="J33" s="139"/>
+      <c r="G33" s="140"/>
+      <c r="H33" s="140"/>
+      <c r="I33" s="140"/>
+      <c r="J33" s="140"/>
     </row>
     <row r="34" spans="1:10" ht="17.25">
       <c r="A34" s="97"/>
@@ -4502,10 +4507,10 @@
       <c r="D34" s="34"/>
       <c r="E34" s="34"/>
       <c r="F34" s="34"/>
-      <c r="G34" s="139"/>
-      <c r="H34" s="139"/>
-      <c r="I34" s="139"/>
-      <c r="J34" s="139"/>
+      <c r="G34" s="140"/>
+      <c r="H34" s="140"/>
+      <c r="I34" s="140"/>
+      <c r="J34" s="140"/>
     </row>
     <row r="35" spans="1:10" ht="17.25">
       <c r="A35" s="98"/>
@@ -4514,10 +4519,10 @@
       <c r="D35" s="34"/>
       <c r="E35" s="34"/>
       <c r="F35" s="34"/>
-      <c r="G35" s="139"/>
-      <c r="H35" s="139"/>
-      <c r="I35" s="139"/>
-      <c r="J35" s="139"/>
+      <c r="G35" s="140"/>
+      <c r="H35" s="140"/>
+      <c r="I35" s="140"/>
+      <c r="J35" s="140"/>
     </row>
     <row r="36" spans="1:10" ht="17.25">
       <c r="A36" s="100"/>
@@ -4526,10 +4531,10 @@
       <c r="D36" s="34"/>
       <c r="E36" s="34"/>
       <c r="F36" s="34"/>
-      <c r="G36" s="139"/>
-      <c r="H36" s="139"/>
-      <c r="I36" s="139"/>
-      <c r="J36" s="139"/>
+      <c r="G36" s="140"/>
+      <c r="H36" s="140"/>
+      <c r="I36" s="140"/>
+      <c r="J36" s="140"/>
     </row>
     <row r="37" spans="1:10" ht="17.25">
       <c r="A37" s="101"/>
@@ -4538,10 +4543,10 @@
       <c r="D37" s="34"/>
       <c r="E37" s="34"/>
       <c r="F37" s="34"/>
-      <c r="G37" s="139"/>
-      <c r="H37" s="139"/>
-      <c r="I37" s="139"/>
-      <c r="J37" s="139"/>
+      <c r="G37" s="140"/>
+      <c r="H37" s="140"/>
+      <c r="I37" s="140"/>
+      <c r="J37" s="140"/>
     </row>
     <row r="38" spans="1:10" ht="17.25">
       <c r="A38" s="34"/>
@@ -4626,8 +4631,8 @@
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
-      <c r="E48" s="151"/>
-      <c r="F48" s="151"/>
+      <c r="E48" s="155"/>
+      <c r="F48" s="155"/>
     </row>
     <row r="50" spans="1:19" ht="17.25">
       <c r="E50" s="37"/>
@@ -4657,14 +4662,14 @@
       <c r="F59" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="G59" s="145" t="s">
+      <c r="G59" s="142" t="s">
         <v>5</v>
       </c>
-      <c r="H59" s="145"/>
-      <c r="I59" s="145" t="s">
+      <c r="H59" s="142"/>
+      <c r="I59" s="142" t="s">
         <v>110</v>
       </c>
-      <c r="J59" s="145"/>
+      <c r="J59" s="142"/>
       <c r="L59" s="2" t="s">
         <v>16</v>
       </c>
@@ -4691,7 +4696,7 @@
       </c>
     </row>
     <row r="60" spans="1:19" ht="17.25">
-      <c r="A60" s="146" t="s">
+      <c r="A60" s="156" t="s">
         <v>111</v>
       </c>
       <c r="B60" s="9"/>
@@ -4705,10 +4710,10 @@
         <v>141</v>
       </c>
       <c r="F60" s="9"/>
-      <c r="G60" s="147"/>
-      <c r="H60" s="147"/>
-      <c r="I60" s="147"/>
-      <c r="J60" s="147"/>
+      <c r="G60" s="153"/>
+      <c r="H60" s="153"/>
+      <c r="I60" s="153"/>
+      <c r="J60" s="153"/>
       <c r="L60" s="3" t="s">
         <v>215</v>
       </c>
@@ -4735,7 +4740,7 @@
       </c>
     </row>
     <row r="61" spans="1:19" ht="17.25">
-      <c r="A61" s="146"/>
+      <c r="A61" s="156"/>
       <c r="B61" s="9"/>
       <c r="C61" s="9" t="s">
         <v>96</v>
@@ -4747,10 +4752,10 @@
         <v>141</v>
       </c>
       <c r="F61" s="9"/>
-      <c r="G61" s="147"/>
-      <c r="H61" s="147"/>
-      <c r="I61" s="147"/>
-      <c r="J61" s="147"/>
+      <c r="G61" s="153"/>
+      <c r="H61" s="153"/>
+      <c r="I61" s="153"/>
+      <c r="J61" s="153"/>
       <c r="L61" s="3" t="s">
         <v>216</v>
       </c>
@@ -4777,7 +4782,7 @@
       </c>
     </row>
     <row r="62" spans="1:19" ht="17.25">
-      <c r="A62" s="146"/>
+      <c r="A62" s="156"/>
       <c r="B62" s="9"/>
       <c r="C62" s="9" t="s">
         <v>97</v>
@@ -4789,10 +4794,10 @@
         <v>141</v>
       </c>
       <c r="F62" s="9"/>
-      <c r="G62" s="147"/>
-      <c r="H62" s="147"/>
-      <c r="I62" s="147"/>
-      <c r="J62" s="147"/>
+      <c r="G62" s="153"/>
+      <c r="H62" s="153"/>
+      <c r="I62" s="153"/>
+      <c r="J62" s="153"/>
       <c r="L62" s="3" t="s">
         <v>285</v>
       </c>
@@ -4819,7 +4824,7 @@
       </c>
     </row>
     <row r="63" spans="1:19" ht="17.25">
-      <c r="A63" s="148" t="s">
+      <c r="A63" s="154" t="s">
         <v>284</v>
       </c>
       <c r="B63" s="10"/>
@@ -4835,10 +4840,10 @@
       <c r="F63" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="G63" s="152"/>
-      <c r="H63" s="152"/>
-      <c r="I63" s="152"/>
-      <c r="J63" s="152"/>
+      <c r="G63" s="150"/>
+      <c r="H63" s="150"/>
+      <c r="I63" s="150"/>
+      <c r="J63" s="150"/>
       <c r="L63" s="3" t="s">
         <v>282</v>
       </c>
@@ -4865,7 +4870,7 @@
       </c>
     </row>
     <row r="64" spans="1:19" ht="17.25">
-      <c r="A64" s="148"/>
+      <c r="A64" s="154"/>
       <c r="B64" s="10"/>
       <c r="C64" s="10" t="s">
         <v>98</v>
@@ -4909,7 +4914,7 @@
       </c>
     </row>
     <row r="65" spans="1:19" ht="17.25">
-      <c r="A65" s="148"/>
+      <c r="A65" s="154"/>
       <c r="B65" s="10"/>
       <c r="C65" s="10" t="s">
         <v>182</v>
@@ -4969,10 +4974,10 @@
       <c r="F66" s="35" t="s">
         <v>239</v>
       </c>
-      <c r="G66" s="142"/>
-      <c r="H66" s="142"/>
-      <c r="I66" s="142"/>
-      <c r="J66" s="142"/>
+      <c r="G66" s="151"/>
+      <c r="H66" s="151"/>
+      <c r="I66" s="151"/>
+      <c r="J66" s="151"/>
       <c r="L66" s="3"/>
       <c r="M66" s="4"/>
       <c r="N66" s="4"/>
@@ -4999,10 +5004,10 @@
       <c r="F67" s="71" t="s">
         <v>239</v>
       </c>
-      <c r="G67" s="153"/>
-      <c r="H67" s="153"/>
-      <c r="I67" s="153"/>
-      <c r="J67" s="153"/>
+      <c r="G67" s="139"/>
+      <c r="H67" s="139"/>
+      <c r="I67" s="139"/>
+      <c r="J67" s="139"/>
       <c r="L67" s="3"/>
       <c r="M67" s="4"/>
       <c r="N67" s="4"/>
@@ -5029,10 +5034,10 @@
       <c r="F68" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="G68" s="154"/>
-      <c r="H68" s="154"/>
-      <c r="I68" s="154"/>
-      <c r="J68" s="154"/>
+      <c r="G68" s="152"/>
+      <c r="H68" s="152"/>
+      <c r="I68" s="152"/>
+      <c r="J68" s="152"/>
       <c r="S68" s="4"/>
     </row>
     <row r="69" spans="1:19" ht="17.25">
@@ -5260,10 +5265,10 @@
       <c r="F76" s="77" t="s">
         <v>239</v>
       </c>
-      <c r="G76" s="140"/>
-      <c r="H76" s="140"/>
-      <c r="I76" s="140"/>
-      <c r="J76" s="140"/>
+      <c r="G76" s="149"/>
+      <c r="H76" s="149"/>
+      <c r="I76" s="149"/>
+      <c r="J76" s="149"/>
     </row>
     <row r="77" spans="1:19" ht="18" thickBot="1">
       <c r="A77" s="79" t="s">
@@ -5284,10 +5289,10 @@
       <c r="F77" s="81" t="s">
         <v>239</v>
       </c>
-      <c r="G77" s="141"/>
-      <c r="H77" s="141"/>
-      <c r="I77" s="141"/>
-      <c r="J77" s="141"/>
+      <c r="G77" s="146"/>
+      <c r="H77" s="146"/>
+      <c r="I77" s="146"/>
+      <c r="J77" s="146"/>
     </row>
     <row r="78" spans="1:19" ht="17.25">
       <c r="A78" s="82" t="s">
@@ -5306,10 +5311,10 @@
         <v>221</v>
       </c>
       <c r="F78" s="84"/>
-      <c r="G78" s="149"/>
-      <c r="H78" s="149"/>
-      <c r="I78" s="149"/>
-      <c r="J78" s="150"/>
+      <c r="G78" s="147"/>
+      <c r="H78" s="147"/>
+      <c r="I78" s="147"/>
+      <c r="J78" s="148"/>
     </row>
     <row r="79" spans="1:19" ht="17.25">
       <c r="A79" s="85">
@@ -5328,10 +5333,10 @@
         <v>223</v>
       </c>
       <c r="F79" s="1"/>
-      <c r="G79" s="139"/>
-      <c r="H79" s="139"/>
-      <c r="I79" s="139"/>
-      <c r="J79" s="158"/>
+      <c r="G79" s="140"/>
+      <c r="H79" s="140"/>
+      <c r="I79" s="140"/>
+      <c r="J79" s="141"/>
     </row>
     <row r="80" spans="1:19" ht="17.25">
       <c r="A80" s="85">
@@ -5350,10 +5355,10 @@
         <v>224</v>
       </c>
       <c r="F80" s="1"/>
-      <c r="G80" s="139"/>
-      <c r="H80" s="139"/>
-      <c r="I80" s="139"/>
-      <c r="J80" s="158"/>
+      <c r="G80" s="140"/>
+      <c r="H80" s="140"/>
+      <c r="I80" s="140"/>
+      <c r="J80" s="141"/>
     </row>
     <row r="81" spans="1:10" ht="18" thickBot="1">
       <c r="A81" s="86">
@@ -5368,65 +5373,35 @@
       <c r="D81" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="E81" s="155" t="s">
+      <c r="E81" s="143" t="s">
         <v>227</v>
       </c>
-      <c r="F81" s="155"/>
-      <c r="G81" s="156"/>
-      <c r="H81" s="156"/>
-      <c r="I81" s="156"/>
-      <c r="J81" s="157"/>
+      <c r="F81" s="143"/>
+      <c r="G81" s="144"/>
+      <c r="H81" s="144"/>
+      <c r="I81" s="144"/>
+      <c r="J81" s="145"/>
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="G80:H80"/>
-    <mergeCell ref="I80:J80"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="E81:F81"/>
-    <mergeCell ref="G81:H81"/>
-    <mergeCell ref="I81:J81"/>
-    <mergeCell ref="G77:H77"/>
-    <mergeCell ref="I77:J77"/>
-    <mergeCell ref="G78:H78"/>
-    <mergeCell ref="I78:J78"/>
-    <mergeCell ref="G79:H79"/>
-    <mergeCell ref="I79:J79"/>
-    <mergeCell ref="G76:H76"/>
-    <mergeCell ref="I76:J76"/>
-    <mergeCell ref="G63:H63"/>
-    <mergeCell ref="I63:J63"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="I67:J67"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="I68:J68"/>
-    <mergeCell ref="I60:J60"/>
-    <mergeCell ref="G61:H61"/>
-    <mergeCell ref="I61:J61"/>
-    <mergeCell ref="G62:H62"/>
-    <mergeCell ref="I62:J62"/>
-    <mergeCell ref="A63:A65"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I24:J24"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="A1:J1"/>
@@ -5443,24 +5418,54 @@
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="I22:J22"/>
     <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="I60:J60"/>
+    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="I61:J61"/>
+    <mergeCell ref="G62:H62"/>
+    <mergeCell ref="I62:J62"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="I67:J67"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="I68:J68"/>
+    <mergeCell ref="E81:F81"/>
+    <mergeCell ref="G81:H81"/>
+    <mergeCell ref="I81:J81"/>
+    <mergeCell ref="G77:H77"/>
+    <mergeCell ref="I77:J77"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="I78:J78"/>
+    <mergeCell ref="G79:H79"/>
+    <mergeCell ref="I79:J79"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="G80:H80"/>
+    <mergeCell ref="I80:J80"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="G76:H76"/>
+    <mergeCell ref="I76:J76"/>
+    <mergeCell ref="G63:H63"/>
+    <mergeCell ref="I63:J63"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5472,8 +5477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27F8DC3-BDE0-43F3-979D-2CCDC5541D2C}">
   <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView topLeftCell="E4" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -5497,14 +5502,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="167" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
+      <c r="B1" s="168"/>
+      <c r="C1" s="168"/>
+      <c r="D1" s="168"/>
+      <c r="E1" s="168"/>
+      <c r="F1" s="168"/>
     </row>
     <row r="2" spans="1:20" ht="37.5">
       <c r="A2" s="42" t="s">
@@ -5525,17 +5530,17 @@
       <c r="F2" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="164" t="s">
+      <c r="G2" s="169" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="164"/>
-      <c r="I2" s="164" t="s">
+      <c r="H2" s="169"/>
+      <c r="I2" s="169" t="s">
         <v>110</v>
       </c>
-      <c r="J2" s="164"/>
+      <c r="J2" s="169"/>
     </row>
     <row r="3" spans="1:20" ht="36">
-      <c r="A3" s="159" t="s">
+      <c r="A3" s="170" t="s">
         <v>81</v>
       </c>
       <c r="B3" s="43"/>
@@ -5549,10 +5554,10 @@
         <v>141</v>
       </c>
       <c r="F3" s="43"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="161"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="161"/>
+      <c r="G3" s="159"/>
+      <c r="H3" s="160"/>
+      <c r="I3" s="159"/>
+      <c r="J3" s="160"/>
       <c r="L3" s="41" t="s">
         <v>58</v>
       </c>
@@ -5565,7 +5570,7 @@
       <c r="S3" s="46"/>
     </row>
     <row r="4" spans="1:20" ht="36">
-      <c r="A4" s="159"/>
+      <c r="A4" s="170"/>
       <c r="B4" s="43"/>
       <c r="C4" s="44" t="s">
         <v>189</v>
@@ -5577,10 +5582,10 @@
         <v>141</v>
       </c>
       <c r="F4" s="43"/>
-      <c r="G4" s="160"/>
-      <c r="H4" s="161"/>
-      <c r="I4" s="160"/>
-      <c r="J4" s="161"/>
+      <c r="G4" s="159"/>
+      <c r="H4" s="160"/>
+      <c r="I4" s="159"/>
+      <c r="J4" s="160"/>
       <c r="L4" s="48" t="s">
         <v>16</v>
       </c>
@@ -5610,7 +5615,7 @@
       </c>
     </row>
     <row r="5" spans="1:20" ht="75">
-      <c r="A5" s="159"/>
+      <c r="A5" s="170"/>
       <c r="B5" s="43"/>
       <c r="C5" s="50" t="s">
         <v>98</v>
@@ -5655,7 +5660,7 @@
       </c>
     </row>
     <row r="6" spans="1:20" ht="75">
-      <c r="A6" s="159"/>
+      <c r="A6" s="170"/>
       <c r="B6" s="43"/>
       <c r="C6" s="50" t="s">
         <v>97</v>
@@ -5667,10 +5672,10 @@
         <v>27</v>
       </c>
       <c r="F6" s="43"/>
-      <c r="G6" s="160"/>
-      <c r="H6" s="161"/>
-      <c r="I6" s="160"/>
-      <c r="J6" s="161"/>
+      <c r="G6" s="159"/>
+      <c r="H6" s="160"/>
+      <c r="I6" s="159"/>
+      <c r="J6" s="160"/>
       <c r="L6" s="54" t="s">
         <v>62</v>
       </c>
@@ -5700,7 +5705,7 @@
       </c>
     </row>
     <row r="7" spans="1:20" ht="75">
-      <c r="A7" s="165" t="s">
+      <c r="A7" s="164" t="s">
         <v>82</v>
       </c>
       <c r="B7" s="43"/>
@@ -5714,10 +5719,10 @@
         <v>27</v>
       </c>
       <c r="F7" s="51"/>
-      <c r="G7" s="160"/>
-      <c r="H7" s="161"/>
-      <c r="I7" s="160"/>
-      <c r="J7" s="161"/>
+      <c r="G7" s="159"/>
+      <c r="H7" s="160"/>
+      <c r="I7" s="159"/>
+      <c r="J7" s="160"/>
       <c r="L7" s="54" t="s">
         <v>65</v>
       </c>
@@ -5747,7 +5752,7 @@
       </c>
     </row>
     <row r="8" spans="1:20" ht="75">
-      <c r="A8" s="166"/>
+      <c r="A8" s="165"/>
       <c r="B8" s="43"/>
       <c r="C8" s="50" t="s">
         <v>98</v>
@@ -5792,7 +5797,7 @@
       </c>
     </row>
     <row r="9" spans="1:20" ht="75">
-      <c r="A9" s="167"/>
+      <c r="A9" s="166"/>
       <c r="B9" s="43"/>
       <c r="C9" s="50" t="s">
         <v>182</v>
@@ -5837,7 +5842,7 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="37.5">
-      <c r="A10" s="159" t="s">
+      <c r="A10" s="170" t="s">
         <v>83</v>
       </c>
       <c r="B10" s="43"/>
@@ -5851,10 +5856,10 @@
         <v>27</v>
       </c>
       <c r="F10" s="51"/>
-      <c r="G10" s="160"/>
-      <c r="H10" s="161"/>
-      <c r="I10" s="160"/>
-      <c r="J10" s="161"/>
+      <c r="G10" s="159"/>
+      <c r="H10" s="160"/>
+      <c r="I10" s="159"/>
+      <c r="J10" s="160"/>
       <c r="L10" s="54" t="s">
         <v>72</v>
       </c>
@@ -5884,7 +5889,7 @@
       </c>
     </row>
     <row r="11" spans="1:20" ht="56.25">
-      <c r="A11" s="159"/>
+      <c r="A11" s="170"/>
       <c r="B11" s="43"/>
       <c r="C11" s="44" t="s">
         <v>98</v>
@@ -5896,10 +5901,10 @@
         <v>27</v>
       </c>
       <c r="F11" s="56"/>
-      <c r="G11" s="160"/>
-      <c r="H11" s="161"/>
-      <c r="I11" s="160"/>
-      <c r="J11" s="161"/>
+      <c r="G11" s="159"/>
+      <c r="H11" s="160"/>
+      <c r="I11" s="159"/>
+      <c r="J11" s="160"/>
       <c r="L11" s="54" t="s">
         <v>265</v>
       </c>
@@ -5929,7 +5934,7 @@
       </c>
     </row>
     <row r="12" spans="1:20" ht="37.5">
-      <c r="A12" s="159"/>
+      <c r="A12" s="170"/>
       <c r="B12" s="43"/>
       <c r="C12" s="44" t="s">
         <v>182</v>
@@ -5941,10 +5946,10 @@
         <v>27</v>
       </c>
       <c r="F12" s="56"/>
-      <c r="G12" s="160"/>
-      <c r="H12" s="161"/>
-      <c r="I12" s="160"/>
-      <c r="J12" s="161"/>
+      <c r="G12" s="159"/>
+      <c r="H12" s="160"/>
+      <c r="I12" s="159"/>
+      <c r="J12" s="160"/>
       <c r="L12" s="54" t="s">
         <v>72</v>
       </c>
@@ -5955,7 +5960,7 @@
         <v>62</v>
       </c>
       <c r="O12" s="49" t="s">
-        <v>39</v>
+        <v>342</v>
       </c>
       <c r="P12" s="49" t="s">
         <v>24</v>
@@ -5964,17 +5969,17 @@
         <v>25</v>
       </c>
       <c r="R12" s="49" t="s">
-        <v>313</v>
+        <v>343</v>
       </c>
       <c r="S12" s="49" t="s">
-        <v>44</v>
+        <v>344</v>
       </c>
       <c r="T12" s="49" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="168" t="s">
+      <c r="A13" s="161" t="s">
         <v>267</v>
       </c>
       <c r="B13" s="59"/>
@@ -5991,7 +5996,7 @@
       <c r="T13" s="58"/>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="169"/>
+      <c r="A14" s="162"/>
       <c r="B14" s="59"/>
       <c r="C14" s="59" t="s">
         <v>269</v>
@@ -6006,7 +6011,7 @@
       <c r="T14" s="58"/>
     </row>
     <row r="15" spans="1:20" ht="37.5">
-      <c r="A15" s="169"/>
+      <c r="A15" s="162"/>
       <c r="B15" s="59"/>
       <c r="C15" s="62" t="s">
         <v>270</v>
@@ -6025,7 +6030,7 @@
       <c r="T15" s="58"/>
     </row>
     <row r="16" spans="1:20" ht="37.5">
-      <c r="A16" s="169"/>
+      <c r="A16" s="162"/>
       <c r="B16" s="60" t="s">
         <v>108</v>
       </c>
@@ -6044,7 +6049,7 @@
       <c r="T16" s="58"/>
     </row>
     <row r="17" spans="1:19" ht="37.5">
-      <c r="A17" s="170"/>
+      <c r="A17" s="163"/>
       <c r="B17" s="60" t="s">
         <v>107</v>
       </c>
@@ -6071,7 +6076,7 @@
       </c>
     </row>
     <row r="18" spans="1:19">
-      <c r="A18" s="168" t="s">
+      <c r="A18" s="161" t="s">
         <v>276</v>
       </c>
       <c r="B18" s="59"/>
@@ -6097,7 +6102,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" ht="37.5">
-      <c r="A19" s="169"/>
+      <c r="A19" s="162"/>
       <c r="B19" s="59"/>
       <c r="C19" s="59" t="s">
         <v>269</v>
@@ -6121,7 +6126,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" ht="37.5">
-      <c r="A20" s="169"/>
+      <c r="A20" s="162"/>
       <c r="B20" s="59"/>
       <c r="C20" s="59" t="s">
         <v>270</v>
@@ -6149,7 +6154,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" ht="37.5">
-      <c r="A21" s="169"/>
+      <c r="A21" s="162"/>
       <c r="B21" s="60" t="s">
         <v>108</v>
       </c>
@@ -6169,7 +6174,7 @@
       <c r="O21" s="57"/>
     </row>
     <row r="22" spans="1:19" ht="37.5">
-      <c r="A22" s="170"/>
+      <c r="A22" s="163"/>
       <c r="B22" s="60" t="s">
         <v>107</v>
       </c>
@@ -6199,7 +6204,7 @@
       </c>
     </row>
     <row r="23" spans="1:19">
-      <c r="A23" s="165" t="s">
+      <c r="A23" s="164" t="s">
         <v>84</v>
       </c>
       <c r="B23" s="43"/>
@@ -6209,10 +6214,10 @@
       <c r="D23" s="51"/>
       <c r="E23" s="51"/>
       <c r="F23" s="56"/>
-      <c r="G23" s="160"/>
-      <c r="H23" s="161"/>
-      <c r="I23" s="160"/>
-      <c r="J23" s="161"/>
+      <c r="G23" s="159"/>
+      <c r="H23" s="160"/>
+      <c r="I23" s="159"/>
+      <c r="J23" s="160"/>
       <c r="L23" s="60" t="s">
         <v>107</v>
       </c>
@@ -6231,7 +6236,7 @@
       <c r="S23" s="58"/>
     </row>
     <row r="24" spans="1:19">
-      <c r="A24" s="166"/>
+      <c r="A24" s="165"/>
       <c r="B24" s="43"/>
       <c r="C24" s="50" t="s">
         <v>99</v>
@@ -6239,14 +6244,14 @@
       <c r="D24" s="51"/>
       <c r="E24" s="51"/>
       <c r="F24" s="56"/>
-      <c r="G24" s="160"/>
-      <c r="H24" s="161"/>
-      <c r="I24" s="160"/>
-      <c r="J24" s="161"/>
+      <c r="G24" s="159"/>
+      <c r="H24" s="160"/>
+      <c r="I24" s="159"/>
+      <c r="J24" s="160"/>
       <c r="M24" s="64"/>
     </row>
     <row r="25" spans="1:19">
-      <c r="A25" s="166"/>
+      <c r="A25" s="165"/>
       <c r="B25" s="43"/>
       <c r="C25" s="50" t="s">
         <v>100</v>
@@ -6254,10 +6259,10 @@
       <c r="D25" s="51"/>
       <c r="E25" s="51"/>
       <c r="F25" s="56"/>
-      <c r="G25" s="160"/>
-      <c r="H25" s="161"/>
-      <c r="I25" s="160"/>
-      <c r="J25" s="161"/>
+      <c r="G25" s="159"/>
+      <c r="H25" s="160"/>
+      <c r="I25" s="159"/>
+      <c r="J25" s="160"/>
       <c r="L25" s="60" t="s">
         <v>108</v>
       </c>
@@ -6272,7 +6277,7 @@
       </c>
     </row>
     <row r="26" spans="1:19">
-      <c r="A26" s="166"/>
+      <c r="A26" s="165"/>
       <c r="B26" s="43"/>
       <c r="C26" s="50" t="s">
         <v>101</v>
@@ -6280,10 +6285,10 @@
       <c r="D26" s="51"/>
       <c r="E26" s="51"/>
       <c r="F26" s="51"/>
-      <c r="G26" s="160"/>
-      <c r="H26" s="161"/>
-      <c r="I26" s="160"/>
-      <c r="J26" s="161"/>
+      <c r="G26" s="159"/>
+      <c r="H26" s="160"/>
+      <c r="I26" s="159"/>
+      <c r="J26" s="160"/>
       <c r="L26" s="60" t="s">
         <v>107</v>
       </c>
@@ -6298,7 +6303,7 @@
       </c>
     </row>
     <row r="27" spans="1:19">
-      <c r="A27" s="166"/>
+      <c r="A27" s="165"/>
       <c r="B27" s="43"/>
       <c r="C27" s="50" t="s">
         <v>102</v>
@@ -6306,13 +6311,13 @@
       <c r="D27" s="51"/>
       <c r="E27" s="51"/>
       <c r="F27" s="51"/>
-      <c r="G27" s="160"/>
-      <c r="H27" s="161"/>
-      <c r="I27" s="160"/>
-      <c r="J27" s="161"/>
+      <c r="G27" s="159"/>
+      <c r="H27" s="160"/>
+      <c r="I27" s="159"/>
+      <c r="J27" s="160"/>
     </row>
     <row r="28" spans="1:19">
-      <c r="A28" s="166"/>
+      <c r="A28" s="165"/>
       <c r="B28" s="43"/>
       <c r="C28" s="50" t="s">
         <v>103</v>
@@ -6320,13 +6325,13 @@
       <c r="D28" s="51"/>
       <c r="E28" s="51"/>
       <c r="F28" s="51"/>
-      <c r="G28" s="160"/>
-      <c r="H28" s="161"/>
-      <c r="I28" s="160"/>
-      <c r="J28" s="161"/>
+      <c r="G28" s="159"/>
+      <c r="H28" s="160"/>
+      <c r="I28" s="159"/>
+      <c r="J28" s="160"/>
     </row>
     <row r="29" spans="1:19">
-      <c r="A29" s="166"/>
+      <c r="A29" s="165"/>
       <c r="B29" s="43"/>
       <c r="C29" s="50" t="s">
         <v>104</v>
@@ -6340,19 +6345,19 @@
       <c r="J29" s="53"/>
     </row>
     <row r="30" spans="1:19">
-      <c r="A30" s="167"/>
+      <c r="A30" s="166"/>
       <c r="B30" s="59" t="s">
         <v>109</v>
       </c>
       <c r="D30" s="51"/>
       <c r="E30" s="51"/>
-      <c r="G30" s="160"/>
-      <c r="H30" s="161"/>
-      <c r="I30" s="160"/>
-      <c r="J30" s="161"/>
+      <c r="G30" s="159"/>
+      <c r="H30" s="160"/>
+      <c r="I30" s="159"/>
+      <c r="J30" s="160"/>
     </row>
     <row r="31" spans="1:19">
-      <c r="A31" s="168" t="s">
+      <c r="A31" s="161" t="s">
         <v>85</v>
       </c>
       <c r="B31" s="65"/>
@@ -6362,13 +6367,13 @@
       <c r="D31" s="51"/>
       <c r="E31" s="51"/>
       <c r="F31" s="51"/>
-      <c r="G31" s="160"/>
-      <c r="H31" s="161"/>
-      <c r="I31" s="160"/>
-      <c r="J31" s="161"/>
+      <c r="G31" s="159"/>
+      <c r="H31" s="160"/>
+      <c r="I31" s="159"/>
+      <c r="J31" s="160"/>
     </row>
     <row r="32" spans="1:19">
-      <c r="A32" s="169"/>
+      <c r="A32" s="162"/>
       <c r="B32" s="65"/>
       <c r="C32" s="50" t="s">
         <v>99</v>
@@ -6376,13 +6381,13 @@
       <c r="D32" s="51"/>
       <c r="E32" s="51"/>
       <c r="F32" s="51"/>
-      <c r="G32" s="160"/>
-      <c r="H32" s="161"/>
-      <c r="I32" s="160"/>
-      <c r="J32" s="161"/>
+      <c r="G32" s="159"/>
+      <c r="H32" s="160"/>
+      <c r="I32" s="159"/>
+      <c r="J32" s="160"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="169"/>
+      <c r="A33" s="162"/>
       <c r="B33" s="65"/>
       <c r="C33" s="50" t="s">
         <v>100</v>
@@ -6390,13 +6395,13 @@
       <c r="D33" s="51"/>
       <c r="E33" s="51"/>
       <c r="F33" s="51"/>
-      <c r="G33" s="160"/>
-      <c r="H33" s="161"/>
-      <c r="I33" s="160"/>
-      <c r="J33" s="161"/>
+      <c r="G33" s="159"/>
+      <c r="H33" s="160"/>
+      <c r="I33" s="159"/>
+      <c r="J33" s="160"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="169"/>
+      <c r="A34" s="162"/>
       <c r="B34" s="65"/>
       <c r="C34" s="50" t="s">
         <v>101</v>
@@ -6404,13 +6409,13 @@
       <c r="D34" s="51"/>
       <c r="E34" s="51"/>
       <c r="F34" s="51"/>
-      <c r="G34" s="160"/>
-      <c r="H34" s="161"/>
-      <c r="I34" s="160"/>
-      <c r="J34" s="161"/>
+      <c r="G34" s="159"/>
+      <c r="H34" s="160"/>
+      <c r="I34" s="159"/>
+      <c r="J34" s="160"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="169"/>
+      <c r="A35" s="162"/>
       <c r="B35" s="65"/>
       <c r="C35" s="50" t="s">
         <v>102</v>
@@ -6418,13 +6423,13 @@
       <c r="D35" s="51"/>
       <c r="E35" s="51"/>
       <c r="F35" s="51"/>
-      <c r="G35" s="160"/>
-      <c r="H35" s="161"/>
-      <c r="I35" s="160"/>
-      <c r="J35" s="161"/>
+      <c r="G35" s="159"/>
+      <c r="H35" s="160"/>
+      <c r="I35" s="159"/>
+      <c r="J35" s="160"/>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="169"/>
+      <c r="A36" s="162"/>
       <c r="B36" s="65"/>
       <c r="C36" s="50" t="s">
         <v>103</v>
@@ -6432,13 +6437,13 @@
       <c r="D36" s="51"/>
       <c r="E36" s="51"/>
       <c r="F36" s="51"/>
-      <c r="G36" s="160"/>
-      <c r="H36" s="161"/>
-      <c r="I36" s="160"/>
-      <c r="J36" s="161"/>
+      <c r="G36" s="159"/>
+      <c r="H36" s="160"/>
+      <c r="I36" s="159"/>
+      <c r="J36" s="160"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="169"/>
+      <c r="A37" s="162"/>
       <c r="B37" s="65"/>
       <c r="C37" s="50" t="s">
         <v>104</v>
@@ -6446,13 +6451,13 @@
       <c r="D37" s="51"/>
       <c r="E37" s="51"/>
       <c r="F37" s="51"/>
-      <c r="G37" s="160"/>
-      <c r="H37" s="161"/>
-      <c r="I37" s="160"/>
-      <c r="J37" s="161"/>
+      <c r="G37" s="159"/>
+      <c r="H37" s="160"/>
+      <c r="I37" s="159"/>
+      <c r="J37" s="160"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="169"/>
+      <c r="A38" s="162"/>
       <c r="B38" s="65"/>
       <c r="C38" s="50" t="s">
         <v>105</v>
@@ -6466,16 +6471,16 @@
       <c r="J38" s="53"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="170"/>
+      <c r="A39" s="163"/>
       <c r="B39" s="59" t="s">
         <v>109</v>
       </c>
       <c r="D39" s="51"/>
       <c r="E39" s="51"/>
-      <c r="G39" s="160"/>
-      <c r="H39" s="161"/>
-      <c r="I39" s="160"/>
-      <c r="J39" s="161"/>
+      <c r="G39" s="159"/>
+      <c r="H39" s="160"/>
+      <c r="I39" s="159"/>
+      <c r="J39" s="160"/>
     </row>
     <row r="40" spans="1:10" ht="37.5">
       <c r="A40" s="59" t="s">
@@ -6483,10 +6488,10 @@
       </c>
       <c r="B40" s="59"/>
       <c r="C40" s="59" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D40" s="51" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E40" s="61" t="s">
         <v>25</v>
@@ -6494,10 +6499,10 @@
       <c r="F40" s="61" t="s">
         <v>128</v>
       </c>
-      <c r="G40" s="160"/>
-      <c r="H40" s="161"/>
-      <c r="I40" s="160"/>
-      <c r="J40" s="161"/>
+      <c r="G40" s="159"/>
+      <c r="H40" s="160"/>
+      <c r="I40" s="159"/>
+      <c r="J40" s="160"/>
     </row>
     <row r="41" spans="1:10" ht="37.5">
       <c r="A41" s="59" t="s">
@@ -6516,10 +6521,10 @@
       <c r="F41" s="47" t="s">
         <v>258</v>
       </c>
-      <c r="G41" s="160"/>
-      <c r="H41" s="161"/>
-      <c r="I41" s="160"/>
-      <c r="J41" s="161"/>
+      <c r="G41" s="159"/>
+      <c r="H41" s="160"/>
+      <c r="I41" s="159"/>
+      <c r="J41" s="160"/>
     </row>
     <row r="42" spans="1:10" ht="37.5">
       <c r="A42" s="59" t="s">
@@ -6540,10 +6545,10 @@
       <c r="F42" s="63" t="s">
         <v>128</v>
       </c>
-      <c r="G42" s="160"/>
-      <c r="H42" s="161"/>
-      <c r="I42" s="160"/>
-      <c r="J42" s="161"/>
+      <c r="G42" s="159"/>
+      <c r="H42" s="160"/>
+      <c r="I42" s="159"/>
+      <c r="J42" s="160"/>
     </row>
     <row r="43" spans="1:10" ht="37.5">
       <c r="A43" s="59" t="s">
@@ -6564,10 +6569,10 @@
       <c r="F43" s="63" t="s">
         <v>128</v>
       </c>
-      <c r="G43" s="160"/>
-      <c r="H43" s="161"/>
-      <c r="I43" s="160"/>
-      <c r="J43" s="161"/>
+      <c r="G43" s="159"/>
+      <c r="H43" s="160"/>
+      <c r="I43" s="159"/>
+      <c r="J43" s="160"/>
     </row>
     <row r="44" spans="1:10" ht="37.5">
       <c r="A44" s="59" t="s">
@@ -6588,10 +6593,10 @@
       <c r="F44" s="63" t="s">
         <v>127</v>
       </c>
-      <c r="G44" s="160"/>
-      <c r="H44" s="161"/>
-      <c r="I44" s="160"/>
-      <c r="J44" s="161"/>
+      <c r="G44" s="159"/>
+      <c r="H44" s="160"/>
+      <c r="I44" s="159"/>
+      <c r="J44" s="160"/>
     </row>
     <row r="45" spans="1:10" ht="37.5">
       <c r="A45" s="59" t="s">
@@ -6612,10 +6617,10 @@
       <c r="F45" s="63" t="s">
         <v>127</v>
       </c>
-      <c r="G45" s="160"/>
-      <c r="H45" s="161"/>
-      <c r="I45" s="160"/>
-      <c r="J45" s="161"/>
+      <c r="G45" s="159"/>
+      <c r="H45" s="160"/>
+      <c r="I45" s="159"/>
+      <c r="J45" s="160"/>
     </row>
     <row r="46" spans="1:10" ht="37.5">
       <c r="A46" s="59" t="s">
@@ -6636,10 +6641,10 @@
       <c r="F46" s="63" t="s">
         <v>127</v>
       </c>
-      <c r="G46" s="160"/>
-      <c r="H46" s="161"/>
-      <c r="I46" s="160"/>
-      <c r="J46" s="161"/>
+      <c r="G46" s="159"/>
+      <c r="H46" s="160"/>
+      <c r="I46" s="159"/>
+      <c r="J46" s="160"/>
     </row>
     <row r="47" spans="1:10" ht="37.5">
       <c r="A47" s="59" t="s">
@@ -6660,10 +6665,10 @@
       <c r="F47" s="63" t="s">
         <v>128</v>
       </c>
-      <c r="G47" s="160"/>
-      <c r="H47" s="161"/>
-      <c r="I47" s="160"/>
-      <c r="J47" s="161"/>
+      <c r="G47" s="159"/>
+      <c r="H47" s="160"/>
+      <c r="I47" s="159"/>
+      <c r="J47" s="160"/>
     </row>
     <row r="48" spans="1:10" ht="37.5">
       <c r="A48" s="59" t="s">
@@ -6672,7 +6677,7 @@
       <c r="B48" s="59"/>
       <c r="C48" s="59"/>
       <c r="D48" s="51" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E48" s="49" t="s">
         <v>25</v>
@@ -6680,10 +6685,10 @@
       <c r="F48" s="51" t="s">
         <v>172</v>
       </c>
-      <c r="G48" s="160"/>
-      <c r="H48" s="161"/>
-      <c r="I48" s="160"/>
-      <c r="J48" s="161"/>
+      <c r="G48" s="159"/>
+      <c r="H48" s="160"/>
+      <c r="I48" s="159"/>
+      <c r="J48" s="160"/>
     </row>
     <row r="49" spans="1:10" ht="37.5">
       <c r="A49" s="59" t="s">
@@ -6692,7 +6697,7 @@
       <c r="B49" s="59"/>
       <c r="C49" s="59"/>
       <c r="D49" s="51" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E49" s="49" t="s">
         <v>25</v>
@@ -6700,10 +6705,10 @@
       <c r="F49" s="51" t="s">
         <v>172</v>
       </c>
-      <c r="G49" s="160"/>
-      <c r="H49" s="161"/>
-      <c r="I49" s="160"/>
-      <c r="J49" s="161"/>
+      <c r="G49" s="159"/>
+      <c r="H49" s="160"/>
+      <c r="I49" s="159"/>
+      <c r="J49" s="160"/>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="59"/>
@@ -6714,27 +6719,66 @@
       <c r="D50" s="59"/>
       <c r="E50" s="59"/>
       <c r="F50" s="59"/>
-      <c r="G50" s="160"/>
-      <c r="H50" s="161"/>
-      <c r="I50" s="160"/>
-      <c r="J50" s="161"/>
+      <c r="G50" s="159"/>
+      <c r="H50" s="160"/>
+      <c r="I50" s="159"/>
+      <c r="J50" s="160"/>
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="A23:A30"/>
+    <mergeCell ref="A31:A39"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G23:H23"/>
     <mergeCell ref="I37:J37"/>
     <mergeCell ref="G39:H39"/>
     <mergeCell ref="I39:J39"/>
@@ -6744,59 +6788,20 @@
     <mergeCell ref="I35:J35"/>
     <mergeCell ref="G36:H36"/>
     <mergeCell ref="I36:J36"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="A23:A30"/>
-    <mergeCell ref="A31:A39"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="I49:J49"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7033,14 +7038,14 @@
       <c r="F11" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="164" t="s">
+      <c r="G11" s="169" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="164"/>
-      <c r="I11" s="164" t="s">
+      <c r="H11" s="169"/>
+      <c r="I11" s="169" t="s">
         <v>110</v>
       </c>
-      <c r="J11" s="164"/>
+      <c r="J11" s="169"/>
     </row>
     <row r="12" spans="1:10" ht="18.75">
       <c r="A12" s="42"/>
@@ -7117,22 +7122,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="110" t="s">
+        <v>317</v>
+      </c>
+      <c r="B1" s="110" t="s">
         <v>318</v>
       </c>
-      <c r="B1" s="110" t="s">
+      <c r="C1" s="110" t="s">
         <v>319</v>
       </c>
-      <c r="C1" s="110" t="s">
+      <c r="D1" s="110" t="s">
         <v>320</v>
       </c>
-      <c r="D1" s="110" t="s">
+      <c r="E1" s="110" t="s">
         <v>321</v>
       </c>
-      <c r="E1" s="110" t="s">
+      <c r="F1" t="s">
         <v>322</v>
-      </c>
-      <c r="F1" t="s">
-        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>